<commit_message>
changed GUI to work with the new Main
</commit_message>
<xml_diff>
--- a/twitter-influencer-ranking/ranking_output.xlsx
+++ b/twitter-influencer-ranking/ranking_output.xlsx
@@ -320,22 +320,52 @@
     <t>@JacobKinge</t>
   </si>
   <si>
+    <t>Everything Georgia</t>
+  </si>
+  <si>
+    <t>@GAFollowers</t>
+  </si>
+  <si>
+    <t>POWR</t>
+  </si>
+  <si>
+    <t>@POWReSports</t>
+  </si>
+  <si>
+    <t>dex</t>
+  </si>
+  <si>
+    <t>@lowkeydex</t>
+  </si>
+  <si>
     <t>Gordon</t>
   </si>
   <si>
     <t>@AltcoinGordon</t>
   </si>
   <si>
+    <t>Revolving Games</t>
+  </si>
+  <si>
+    <t>@Revolving_Games</t>
+  </si>
+  <si>
+    <t>Mnemonics_coin</t>
+  </si>
+  <si>
+    <t>@Mnemonics_coin</t>
+  </si>
+  <si>
     <t>Somos Cosmos</t>
   </si>
   <si>
     <t>@InformaCosmos</t>
   </si>
   <si>
-    <t>dex</t>
-  </si>
-  <si>
-    <t>@lowkeydex</t>
+    <t>Not Jerome Powell</t>
+  </si>
+  <si>
+    <t>@alifarhat79</t>
   </si>
   <si>
     <t>Soompi</t>
@@ -344,40 +374,10 @@
     <t>@soompi</t>
   </si>
   <si>
-    <t>Mnemonics_coin</t>
-  </si>
-  <si>
-    <t>@Mnemonics_coin</t>
-  </si>
-  <si>
-    <t>Revolving Games</t>
-  </si>
-  <si>
-    <t>@Revolving_Games</t>
-  </si>
-  <si>
-    <t>Everything Georgia</t>
-  </si>
-  <si>
-    <t>@GAFollowers</t>
-  </si>
-  <si>
-    <t>POWR</t>
-  </si>
-  <si>
-    <t>@POWReSports</t>
-  </si>
-  <si>
     <t>PepeMeme</t>
   </si>
   <si>
     <t>@PepeMeme_</t>
-  </si>
-  <si>
-    <t>Not Jerome Powell</t>
-  </si>
-  <si>
-    <t>@alifarhat79</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
         <v>1.37E7</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0063818064981122765</v>
+        <v>0.006381806498112274</v>
       </c>
     </row>
     <row r="4">
@@ -513,7 +513,7 @@
         <v>2400000.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0033243519842581894</v>
+        <v>0.00332435198425819</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +533,7 @@
         <v>980000.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.002898211144201299</v>
+        <v>0.0028982111442012984</v>
       </c>
     </row>
     <row r="6">
@@ -553,7 +553,7 @@
         <v>775500.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00272447476279613</v>
+        <v>0.0027244747627961285</v>
       </c>
     </row>
     <row r="7">
@@ -573,7 +573,7 @@
         <v>3400000.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.002707158034597902</v>
+        <v>0.0027071580345979025</v>
       </c>
     </row>
     <row r="8">
@@ -733,7 +733,7 @@
         <v>1000000.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.001984269513633051</v>
+        <v>0.0019842695136330505</v>
       </c>
     </row>
     <row r="16">
@@ -773,7 +773,7 @@
         <v>920900.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0017786097712432385</v>
+        <v>0.0017786097712432381</v>
       </c>
     </row>
     <row r="18">
@@ -833,7 +833,7 @@
         <v>1300000.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0013437347789893887</v>
+        <v>0.0013437347789893891</v>
       </c>
     </row>
     <row r="21">
@@ -853,7 +853,7 @@
         <v>4200000.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0013085925479626496</v>
+        <v>0.0013085925479626491</v>
       </c>
     </row>
     <row r="22">
@@ -873,7 +873,7 @@
         <v>906900.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.001241236740585864</v>
+        <v>0.0012412367405858636</v>
       </c>
     </row>
     <row r="23">
@@ -933,7 +933,7 @@
         <v>629700.0</v>
       </c>
       <c r="F25" t="n">
-        <v>9.736097081617731E-4</v>
+        <v>9.736097081617733E-4</v>
       </c>
     </row>
     <row r="26">
@@ -953,7 +953,7 @@
         <v>2000000.0</v>
       </c>
       <c r="F26" t="n">
-        <v>9.020398400790574E-4</v>
+        <v>9.020398400790572E-4</v>
       </c>
     </row>
     <row r="27">
@@ -973,7 +973,7 @@
         <v>1500000.0</v>
       </c>
       <c r="F27" t="n">
-        <v>8.953283935297853E-4</v>
+        <v>8.953283935297851E-4</v>
       </c>
     </row>
     <row r="28">
@@ -1013,7 +1013,7 @@
         <v>595600.0</v>
       </c>
       <c r="F29" t="n">
-        <v>7.696910001534315E-4</v>
+        <v>7.696910001534317E-4</v>
       </c>
     </row>
     <row r="30">
@@ -1093,7 +1093,7 @@
         <v>643300.0</v>
       </c>
       <c r="F33" t="n">
-        <v>7.124174743690126E-4</v>
+        <v>7.124174743690127E-4</v>
       </c>
     </row>
     <row r="34">
@@ -1193,7 +1193,7 @@
         <v>556100.0</v>
       </c>
       <c r="F38" t="n">
-        <v>3.5709274013806053E-4</v>
+        <v>3.570927401380605E-4</v>
       </c>
     </row>
     <row r="39">
@@ -1421,16 +1421,16 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="n">
-        <v>772.0</v>
+        <v>940.0</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="D50" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="E50" t="n">
-        <v>538500.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="F50" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1441,16 +1441,16 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="n">
-        <v>845.0</v>
+        <v>769.0</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="E51" t="n">
-        <v>1100000.0</v>
+        <v>980800.0</v>
       </c>
       <c r="F51" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1461,16 +1461,16 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="n">
-        <v>852.0</v>
+        <v>978.0</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="E52" t="n">
-        <v>2800000.0</v>
+        <v>1700000.0</v>
       </c>
       <c r="F52" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1481,16 +1481,16 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="n">
-        <v>212.0</v>
+        <v>440.0</v>
       </c>
       <c r="C53" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="D53" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="E53" t="n">
-        <v>953900.0</v>
+        <v>702500.0</v>
       </c>
       <c r="F53" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1501,16 +1501,16 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="n">
-        <v>535.0</v>
+        <v>853.0</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E54" t="n">
-        <v>2800000.0</v>
+        <v>775100.0</v>
       </c>
       <c r="F54" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1561,16 +1561,16 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="n">
-        <v>853.0</v>
+        <v>825.0</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>108</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="E57" t="n">
-        <v>775100.0</v>
+        <v>539400.0</v>
       </c>
       <c r="F57" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1581,16 +1581,16 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="n">
-        <v>189.0</v>
+        <v>268.0</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E58" t="n">
-        <v>3600000.0</v>
+        <v>592100.0</v>
       </c>
       <c r="F58" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1601,16 +1601,16 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="n">
-        <v>495.0</v>
+        <v>331.0</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="E59" t="n">
-        <v>568300.0</v>
+        <v>982300.0</v>
       </c>
       <c r="F59" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1621,16 +1621,16 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="n">
-        <v>331.0</v>
+        <v>495.0</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="E60" t="n">
-        <v>982300.0</v>
+        <v>568300.0</v>
       </c>
       <c r="F60" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1641,16 +1641,16 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="n">
-        <v>12.0</v>
+        <v>212.0</v>
       </c>
       <c r="C61" t="s">
-        <v>18</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="E61" t="n">
-        <v>1700000.0</v>
+        <v>953900.0</v>
       </c>
       <c r="F61" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1661,16 +1661,16 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="n">
-        <v>933.0</v>
+        <v>1022.0</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D62" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E62" t="n">
-        <v>3400000.0</v>
+        <v>1200000.0</v>
       </c>
       <c r="F62" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1681,16 +1681,16 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="n">
-        <v>268.0</v>
+        <v>12.0</v>
       </c>
       <c r="C63" t="s">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="E63" t="n">
-        <v>592100.0</v>
+        <v>1700000.0</v>
       </c>
       <c r="F63" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1701,16 +1701,16 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="n">
-        <v>825.0</v>
+        <v>845.0</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="E64" t="n">
-        <v>539400.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="F64" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1721,16 +1721,16 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="n">
-        <v>978.0</v>
+        <v>535.0</v>
       </c>
       <c r="C65" t="s">
-        <v>114</v>
+        <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>1700000.0</v>
+        <v>2800000.0</v>
       </c>
       <c r="F65" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1741,16 +1741,16 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="n">
-        <v>440.0</v>
+        <v>95.0</v>
       </c>
       <c r="C66" t="s">
-        <v>116</v>
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="E66" t="n">
-        <v>702500.0</v>
+        <v>3000000.0</v>
       </c>
       <c r="F66" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1761,16 +1761,16 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="n">
-        <v>769.0</v>
+        <v>45.0</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="E67" t="n">
-        <v>980800.0</v>
+        <v>543000.0</v>
       </c>
       <c r="F67" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1781,16 +1781,16 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="n">
-        <v>340.0</v>
+        <v>933.0</v>
       </c>
       <c r="C68" t="s">
-        <v>118</v>
+        <v>16</v>
       </c>
       <c r="D68" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="E68" t="n">
-        <v>536100.0</v>
+        <v>3400000.0</v>
       </c>
       <c r="F68" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1801,16 +1801,16 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="n">
-        <v>940.0</v>
+        <v>772.0</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="D69" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="E69" t="n">
-        <v>1000000.0</v>
+        <v>538500.0</v>
       </c>
       <c r="F69" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1821,16 +1821,16 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="n">
-        <v>95.0</v>
+        <v>189.0</v>
       </c>
       <c r="C70" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="D70" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="E70" t="n">
-        <v>3000000.0</v>
+        <v>3600000.0</v>
       </c>
       <c r="F70" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1841,16 +1841,16 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="n">
-        <v>1022.0</v>
+        <v>1054.0</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="D71" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E71" t="n">
-        <v>1200000.0</v>
+        <v>965600.0</v>
       </c>
       <c r="F71" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1861,16 +1861,16 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="n">
-        <v>1054.0</v>
+        <v>340.0</v>
       </c>
       <c r="C72" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="E72" t="n">
-        <v>965600.0</v>
+        <v>536100.0</v>
       </c>
       <c r="F72" t="n">
         <v>1.4137606032045243E-4</v>
@@ -1881,16 +1881,16 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="n">
-        <v>45.0</v>
+        <v>852.0</v>
       </c>
       <c r="C73" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="D73" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E73" t="n">
-        <v>543000.0</v>
+        <v>2800000.0</v>
       </c>
       <c r="F73" t="n">
         <v>1.4137606032045243E-4</v>

</xml_diff>

<commit_message>
added Excel Copy and changed graph loading logic
</commit_message>
<xml_diff>
--- a/twitter-influencer-ranking/ranking_output.xlsx
+++ b/twitter-influencer-ranking/ranking_output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="230">
   <si>
     <t>Rank</t>
   </si>
@@ -32,28 +32,352 @@
     <t>PageRank Score</t>
   </si>
   <si>
+    <t>Elon Musk</t>
+  </si>
+  <si>
+    <t>@elonmusk</t>
+  </si>
+  <si>
+    <t>Department of Government Efficiency</t>
+  </si>
+  <si>
+    <t>@DOGE</t>
+  </si>
+  <si>
+    <t>Solana</t>
+  </si>
+  <si>
+    <t>@solana</t>
+  </si>
+  <si>
+    <t>DEGEN NEWS</t>
+  </si>
+  <si>
+    <t>@DegenerateNews</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>@ton_blockchain</t>
+  </si>
+  <si>
+    <t>The Bearable Bull</t>
+  </si>
+  <si>
+    <t>@thebearablebull</t>
+  </si>
+  <si>
+    <t>Binance</t>
+  </si>
+  <si>
+    <t>@binance</t>
+  </si>
+  <si>
+    <t>David "JoelKatz" Schwartz</t>
+  </si>
+  <si>
+    <t>@JoelKatz</t>
+  </si>
+  <si>
+    <t>WIZZ</t>
+  </si>
+  <si>
+    <t>@CryptoWizardd</t>
+  </si>
+  <si>
+    <t>Altcoin Daily</t>
+  </si>
+  <si>
+    <t>@AltcoinDailyio</t>
+  </si>
+  <si>
+    <t>Brad Garlinghouse</t>
+  </si>
+  <si>
+    <t>@bgarlinghouse</t>
+  </si>
+  <si>
+    <t>Crypto Tony</t>
+  </si>
+  <si>
+    <t>@CryptoTony__</t>
+  </si>
+  <si>
+    <t>punya prasun bajpai</t>
+  </si>
+  <si>
+    <t>@ppbajpai</t>
+  </si>
+  <si>
+    <t>ZachXBT</t>
+  </si>
+  <si>
+    <t>@zachxbt</t>
+  </si>
+  <si>
+    <t>Sergey Nazarov</t>
+  </si>
+  <si>
+    <t>@SergeyNazarov</t>
+  </si>
+  <si>
+    <t>Crypto Rover</t>
+  </si>
+  <si>
+    <t>@rovercrc</t>
+  </si>
+  <si>
+    <t>TechDev</t>
+  </si>
+  <si>
+    <t>@TechDev_52</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>@AltcoinGordon</t>
+  </si>
+  <si>
+    <t>XRPP</t>
+  </si>
+  <si>
+    <t>@XRP_Productions</t>
+  </si>
+  <si>
+    <t>The Moon Show</t>
+  </si>
+  <si>
+    <t>@TheMoonCarl</t>
+  </si>
+  <si>
+    <t>Bitcoin Magazine</t>
+  </si>
+  <si>
+    <t>@BitcoinMagazine</t>
+  </si>
+  <si>
+    <t>Brian Armstrong</t>
+  </si>
+  <si>
+    <t>@brian_armstrong</t>
+  </si>
+  <si>
+    <t>Galxe</t>
+  </si>
+  <si>
+    <t>@Galxe</t>
+  </si>
+  <si>
+    <t>Sandeep (※,※)</t>
+  </si>
+  <si>
+    <t>@sandeepnailwal</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>@cz_binance</t>
+  </si>
+  <si>
+    <t>TRON DAO</t>
+  </si>
+  <si>
+    <t>@trondao</t>
+  </si>
+  <si>
+    <t>Marc Andreessen</t>
+  </si>
+  <si>
+    <t>@pmarca</t>
+  </si>
+  <si>
+    <t>Balaji</t>
+  </si>
+  <si>
+    <t>@balajis</t>
+  </si>
+  <si>
+    <t>Cred</t>
+  </si>
+  <si>
+    <t>@CryptoCred</t>
+  </si>
+  <si>
+    <t>DeFi Princess | Storyteller</t>
+  </si>
+  <si>
+    <t>@defiprincess_</t>
+  </si>
+  <si>
+    <t>Preston Pysh</t>
+  </si>
+  <si>
+    <t>@PrestonPysh</t>
+  </si>
+  <si>
+    <t>H.E. Justin Sun</t>
+  </si>
+  <si>
+    <t>@justinsuntron</t>
+  </si>
+  <si>
+    <t>Dogs Community</t>
+  </si>
+  <si>
+    <t>@realDogsHouse</t>
+  </si>
+  <si>
+    <t>Optimism</t>
+  </si>
+  <si>
+    <t>@Optimism</t>
+  </si>
+  <si>
+    <t>Aethir</t>
+  </si>
+  <si>
+    <t>@AethirCloud</t>
+  </si>
+  <si>
+    <t>Alex Becker</t>
+  </si>
+  <si>
+    <t>@ZssBecker</t>
+  </si>
+  <si>
+    <t>Crypto Tea</t>
+  </si>
+  <si>
+    <t>@CryptoTea_</t>
+  </si>
+  <si>
+    <t>Andrew Tate</t>
+  </si>
+  <si>
+    <t>@Cobratate</t>
+  </si>
+  <si>
+    <t>Mercek</t>
+  </si>
+  <si>
+    <t>@WorldOfMercek</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>@AbstractChain</t>
+  </si>
+  <si>
+    <t>Gate.io</t>
+  </si>
+  <si>
+    <t>@gate_io</t>
+  </si>
+  <si>
+    <t>MEXC</t>
+  </si>
+  <si>
+    <t>@MEXC_Official</t>
+  </si>
+  <si>
+    <t>CRYPTO THRO</t>
+  </si>
+  <si>
+    <t>@CryptoThro</t>
+  </si>
+  <si>
+    <t>Soneium</t>
+  </si>
+  <si>
+    <t>@soneium</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>@america</t>
+  </si>
+  <si>
     <t>Ice Open Network</t>
   </si>
   <si>
     <t>@ice_blockchain</t>
   </si>
   <si>
-    <t>Binance</t>
-  </si>
-  <si>
-    <t>@binance</t>
-  </si>
-  <si>
-    <t>CRYPTO THRO</t>
-  </si>
-  <si>
-    <t>@CryptoThro</t>
-  </si>
-  <si>
-    <t>Bitcoin Magazine</t>
-  </si>
-  <si>
-    <t>@BitcoinMagazine</t>
+    <t>Bitget</t>
+  </si>
+  <si>
+    <t>@bitgetglobal</t>
+  </si>
+  <si>
+    <t>Wormhole</t>
+  </si>
+  <si>
+    <t>@wormhole</t>
+  </si>
+  <si>
+    <t>PancakeSwap</t>
+  </si>
+  <si>
+    <t>@PancakeSwap</t>
+  </si>
+  <si>
+    <t>David Sacks</t>
+  </si>
+  <si>
+    <t>@DavidSacks</t>
+  </si>
+  <si>
+    <t>Coach Bruce (kween/acc)</t>
+  </si>
+  <si>
+    <t>@OX_DAO</t>
+  </si>
+  <si>
+    <t>DeBank</t>
+  </si>
+  <si>
+    <t>@DeBankDeFi</t>
+  </si>
+  <si>
+    <t>KiloEx</t>
+  </si>
+  <si>
+    <t>@KiloEx_perp</t>
+  </si>
+  <si>
+    <t>Ivan on Tech</t>
+  </si>
+  <si>
+    <t>@IvanOnTech</t>
+  </si>
+  <si>
+    <t>HEADBOY</t>
+  </si>
+  <si>
+    <t>@NDIDI_GRAM</t>
+  </si>
+  <si>
+    <t>whale</t>
+  </si>
+  <si>
+    <t>@cardano_whale</t>
+  </si>
+  <si>
+    <t>Wendy O</t>
+  </si>
+  <si>
+    <t>@CryptoWendyO</t>
+  </si>
+  <si>
+    <t>Coinbase</t>
+  </si>
+  <si>
+    <t>@coinbase</t>
   </si>
   <si>
     <t>BNB Chain</t>
@@ -62,22 +386,58 @@
     <t>@BNBCHAIN</t>
   </si>
   <si>
-    <t>Coach Bruce (kween/acc)</t>
-  </si>
-  <si>
-    <t>@OX_DAO</t>
-  </si>
-  <si>
-    <t>Balaji</t>
-  </si>
-  <si>
-    <t>@balajis</t>
-  </si>
-  <si>
-    <t>Sergey Nazarov</t>
-  </si>
-  <si>
-    <t>@SergeyNazarov</t>
+    <t>Ash Crypto</t>
+  </si>
+  <si>
+    <t>@Ashcryptoreal</t>
+  </si>
+  <si>
+    <t>Cluster Protocol</t>
+  </si>
+  <si>
+    <t>@ClusterProtocol</t>
+  </si>
+  <si>
+    <t>Supra</t>
+  </si>
+  <si>
+    <t>@SUPRA_Labs</t>
+  </si>
+  <si>
+    <t>The ₿itcoin Therapist</t>
+  </si>
+  <si>
+    <t>@TheBTCTherapist</t>
+  </si>
+  <si>
+    <t>Nayib Bukele</t>
+  </si>
+  <si>
+    <t>@nayibbukele</t>
+  </si>
+  <si>
+    <t>Jason A. Williams</t>
+  </si>
+  <si>
+    <t>@GoingParabolic</t>
+  </si>
+  <si>
+    <t>Confidential Layer</t>
+  </si>
+  <si>
+    <t>@ConfidentialLyr</t>
+  </si>
+  <si>
+    <t>Stellar</t>
+  </si>
+  <si>
+    <t>@StellarOrg</t>
+  </si>
+  <si>
+    <t>Nature is Amazing</t>
+  </si>
+  <si>
+    <t>@AMAZlNGNATURE</t>
   </si>
   <si>
     <t>Crypto.com</t>
@@ -86,28 +446,124 @@
     <t>@cryptocom</t>
   </si>
   <si>
-    <t>Altcoin Daily</t>
-  </si>
-  <si>
-    <t>@AltcoinDailyio</t>
-  </si>
-  <si>
-    <t>Crypto Rover</t>
-  </si>
-  <si>
-    <t>@rovercrc</t>
-  </si>
-  <si>
-    <t>Confidential Layer</t>
-  </si>
-  <si>
-    <t>@ConfidentialLyr</t>
-  </si>
-  <si>
-    <t>Supra</t>
-  </si>
-  <si>
-    <t>@SUPRA_Labs</t>
+    <t>CyrilXBT</t>
+  </si>
+  <si>
+    <t>@cyrilXBT</t>
+  </si>
+  <si>
+    <t>BITCOINLFG®</t>
+  </si>
+  <si>
+    <t>@bitcoinlfgo</t>
+  </si>
+  <si>
+    <t>Avalanche9000</t>
+  </si>
+  <si>
+    <t>@avax</t>
+  </si>
+  <si>
+    <t>Artyfact</t>
+  </si>
+  <si>
+    <t>@artyfact_game</t>
+  </si>
+  <si>
+    <t>van00sa</t>
+  </si>
+  <si>
+    <t>@van00sa</t>
+  </si>
+  <si>
+    <t>Historic Vids</t>
+  </si>
+  <si>
+    <t>@historyinmemes</t>
+  </si>
+  <si>
+    <t>Jacob King</t>
+  </si>
+  <si>
+    <t>@JacobKinge</t>
+  </si>
+  <si>
+    <t>gaut</t>
+  </si>
+  <si>
+    <t>@0xgaut</t>
+  </si>
+  <si>
+    <t>Baby Doge</t>
+  </si>
+  <si>
+    <t>@BabyDogeCoin</t>
+  </si>
+  <si>
+    <t>Uphold</t>
+  </si>
+  <si>
+    <t>@UpholdInc</t>
+  </si>
+  <si>
+    <t>Lingo</t>
+  </si>
+  <si>
+    <t>@Lingocoins</t>
+  </si>
+  <si>
+    <t>Donald J. Trump News</t>
+  </si>
+  <si>
+    <t>@realTrumpNewsX</t>
+  </si>
+  <si>
+    <t>BFDCoin</t>
+  </si>
+  <si>
+    <t>@BFDCoin</t>
+  </si>
+  <si>
+    <t>xMoney.com</t>
+  </si>
+  <si>
+    <t>@xMoney_com</t>
+  </si>
+  <si>
+    <t>Lex Fridman</t>
+  </si>
+  <si>
+    <t>@lexfridman</t>
+  </si>
+  <si>
+    <t>Mnemonics_coin</t>
+  </si>
+  <si>
+    <t>@Mnemonics_coin</t>
+  </si>
+  <si>
+    <t>DuckChain</t>
+  </si>
+  <si>
+    <t>@Duck_Chain</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>@phantom</t>
+  </si>
+  <si>
+    <t>0xNobler</t>
+  </si>
+  <si>
+    <t>@CryptoNobler</t>
+  </si>
+  <si>
+    <t>MANTRA | Mainnet Live</t>
+  </si>
+  <si>
+    <t>@MANTRA_Chain</t>
   </si>
   <si>
     <t>dubzy</t>
@@ -116,46 +572,118 @@
     <t>@dubzyxbt</t>
   </si>
   <si>
-    <t>Phantom</t>
-  </si>
-  <si>
-    <t>@phantom</t>
-  </si>
-  <si>
-    <t>Soneium</t>
-  </si>
-  <si>
-    <t>@soneium</t>
-  </si>
-  <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>@ton_blockchain</t>
-  </si>
-  <si>
-    <t>The ₿itcoin Therapist</t>
-  </si>
-  <si>
-    <t>@TheBTCTherapist</t>
-  </si>
-  <si>
-    <t>Nature is Amazing</t>
-  </si>
-  <si>
-    <t>@AMAZlNGNATURE</t>
-  </si>
-  <si>
-    <t>Ash Crypto</t>
-  </si>
-  <si>
-    <t>@Ashcryptoreal</t>
-  </si>
-  <si>
-    <t>Wormhole</t>
-  </si>
-  <si>
-    <t>@wormhole</t>
+    <t>Radar</t>
+  </si>
+  <si>
+    <t>@RadarHits</t>
+  </si>
+  <si>
+    <t>Bitget Wallet</t>
+  </si>
+  <si>
+    <t>@BitgetWallet</t>
+  </si>
+  <si>
+    <t>Slingshot DAO</t>
+  </si>
+  <si>
+    <t>@SlingshotDAO</t>
+  </si>
+  <si>
+    <t>Wimar.X</t>
+  </si>
+  <si>
+    <t>@DefiWimar</t>
+  </si>
+  <si>
+    <t>Revolving Games</t>
+  </si>
+  <si>
+    <t>@Revolving_Games</t>
+  </si>
+  <si>
+    <t>Ravish Kumar ᴾᵃʳᵒᵈʸ ©</t>
+  </si>
+  <si>
+    <t>@SirRavishFC</t>
+  </si>
+  <si>
+    <t>हर्ष वर्धन त्रिपाठी</t>
+  </si>
+  <si>
+    <t>@MediaHarshVT</t>
+  </si>
+  <si>
+    <t>Leonidas $DOG</t>
+  </si>
+  <si>
+    <t>@LeonidasNFT</t>
+  </si>
+  <si>
+    <t>Unite</t>
+  </si>
+  <si>
+    <t>@uniteio</t>
+  </si>
+  <si>
+    <t>Saakuru Protocol -</t>
+  </si>
+  <si>
+    <t>@saakuru_labs</t>
+  </si>
+  <si>
+    <t>Not Jerome Powell</t>
+  </si>
+  <si>
+    <t>@alifarhat79</t>
+  </si>
+  <si>
+    <t>Jack Poso</t>
+  </si>
+  <si>
+    <t>@JackPosobiec</t>
+  </si>
+  <si>
+    <t>عبدالعزيز أحمد بغلف</t>
+  </si>
+  <si>
+    <t>@AzizbagBag</t>
+  </si>
+  <si>
+    <t>Astra Nova</t>
+  </si>
+  <si>
+    <t>@Astra__Nova</t>
+  </si>
+  <si>
+    <t>Tari</t>
+  </si>
+  <si>
+    <t>@tari</t>
+  </si>
+  <si>
+    <t>Somos Cosmos</t>
+  </si>
+  <si>
+    <t>@InformaCosmos</t>
+  </si>
+  <si>
+    <t>POWR</t>
+  </si>
+  <si>
+    <t>@POWReSports</t>
+  </si>
+  <si>
+    <t>Peter Schiff</t>
+  </si>
+  <si>
+    <t>@PeterSchiff</t>
+  </si>
+  <si>
+    <t>Everything Georgia</t>
+  </si>
+  <si>
+    <t>@GAFollowers</t>
   </si>
   <si>
     <t>Rami Ismail / رامي</t>
@@ -164,184 +692,10 @@
     <t>@tha_rami</t>
   </si>
   <si>
-    <t>Slingshot DAO</t>
-  </si>
-  <si>
-    <t>@SlingshotDAO</t>
-  </si>
-  <si>
-    <t>Lex Fridman</t>
-  </si>
-  <si>
-    <t>@lexfridman</t>
-  </si>
-  <si>
-    <t>Gordon</t>
-  </si>
-  <si>
-    <t>@AltcoinGordon</t>
-  </si>
-  <si>
-    <t>0xNobler</t>
-  </si>
-  <si>
-    <t>@CryptoNobler</t>
-  </si>
-  <si>
-    <t>DuckChain</t>
-  </si>
-  <si>
-    <t>@Duck_Chain</t>
-  </si>
-  <si>
-    <t>xMoney.com</t>
-  </si>
-  <si>
-    <t>@xMoney_com</t>
-  </si>
-  <si>
-    <t>Crypto Tea</t>
-  </si>
-  <si>
-    <t>@CryptoTea_</t>
-  </si>
-  <si>
-    <t>Unite</t>
-  </si>
-  <si>
-    <t>@uniteio</t>
-  </si>
-  <si>
-    <t>Saakuru Protocol -</t>
-  </si>
-  <si>
-    <t>@saakuru_labs</t>
-  </si>
-  <si>
-    <t>Historic Vids</t>
-  </si>
-  <si>
-    <t>@historyinmemes</t>
-  </si>
-  <si>
-    <t>punya prasun bajpai</t>
-  </si>
-  <si>
-    <t>@ppbajpai</t>
-  </si>
-  <si>
-    <t>Wimar.X</t>
-  </si>
-  <si>
-    <t>@DefiWimar</t>
-  </si>
-  <si>
-    <t>Jason A. Williams</t>
-  </si>
-  <si>
-    <t>@GoingParabolic</t>
-  </si>
-  <si>
-    <t>Tari</t>
-  </si>
-  <si>
-    <t>@tari</t>
-  </si>
-  <si>
-    <t>gaut</t>
-  </si>
-  <si>
-    <t>@0xgaut</t>
-  </si>
-  <si>
-    <t>हर्ष वर्धन त्रिपाठी</t>
-  </si>
-  <si>
-    <t>@MediaHarshVT</t>
-  </si>
-  <si>
-    <t>Abstract</t>
-  </si>
-  <si>
-    <t>@AbstractChain</t>
-  </si>
-  <si>
-    <t>Somos Cosmos</t>
-  </si>
-  <si>
-    <t>@InformaCosmos</t>
-  </si>
-  <si>
-    <t>POWR</t>
-  </si>
-  <si>
-    <t>@POWReSports</t>
-  </si>
-  <si>
-    <t>Peter Schiff</t>
-  </si>
-  <si>
-    <t>@PeterSchiff</t>
-  </si>
-  <si>
-    <t>Revolving Games</t>
-  </si>
-  <si>
-    <t>@Revolving_Games</t>
-  </si>
-  <si>
-    <t>Everything Georgia</t>
-  </si>
-  <si>
-    <t>@GAFollowers</t>
-  </si>
-  <si>
-    <t>Astra Nova</t>
-  </si>
-  <si>
-    <t>@Astra__Nova</t>
-  </si>
-  <si>
     <t>More Perfect Union</t>
   </si>
   <si>
     <t>@MorePerfectUS</t>
-  </si>
-  <si>
-    <t>Leonidas $DOG</t>
-  </si>
-  <si>
-    <t>@LeonidasNFT</t>
-  </si>
-  <si>
-    <t>BFDCoin</t>
-  </si>
-  <si>
-    <t>@BFDCoin</t>
-  </si>
-  <si>
-    <t>Not Jerome Powell</t>
-  </si>
-  <si>
-    <t>@alifarhat79</t>
-  </si>
-  <si>
-    <t>Ravish Kumar ᴾᵃʳᵒᵈʸ ©</t>
-  </si>
-  <si>
-    <t>@SirRavishFC</t>
-  </si>
-  <si>
-    <t>Jacob King</t>
-  </si>
-  <si>
-    <t>@JacobKinge</t>
-  </si>
-  <si>
-    <t>Mnemonics_coin</t>
-  </si>
-  <si>
-    <t>@Mnemonics_coin</t>
   </si>
   <si>
     <t>Arena Games</t>
@@ -392,7 +746,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -400,7 +754,7 @@
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="7.578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="23.6640625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="35.10546875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="19.21875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.55078125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="15.22265625" customWidth="true" bestFit="true"/>
@@ -431,7 +785,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>13.0</v>
+        <v>1062.0</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -440,10 +794,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>2800000.0</v>
+        <v>2.067E8</v>
       </c>
       <c r="F2" t="n">
-        <v>0.007749445199689934</v>
+        <v>0.004783248567557784</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +805,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>706.0</v>
+        <v>1064.0</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -460,10 +814,10 @@
         <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>1.37E7</v>
+        <v>2300000.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0068883134054620486</v>
+        <v>0.004693870929501009</v>
       </c>
     </row>
     <row r="4">
@@ -471,7 +825,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>38.0</v>
+        <v>1085.0</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -480,10 +834,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>154300.0</v>
+        <v>2900000.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0046734274822197285</v>
+        <v>0.004366238061226845</v>
       </c>
     </row>
     <row r="5">
@@ -491,7 +845,7 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="n">
-        <v>10.0</v>
+        <v>1152.0</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -500,10 +854,10 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>3400000.0</v>
+        <v>292300.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.002845735098994946</v>
+        <v>0.004274227260107351</v>
       </c>
     </row>
     <row r="6">
@@ -511,7 +865,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>857.0</v>
+        <v>11.0</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -520,10 +874,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>3600000.0</v>
+        <v>2500000.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.002828019070617323</v>
+        <v>0.00353142275637502</v>
       </c>
     </row>
     <row r="7">
@@ -531,7 +885,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>243.0</v>
+        <v>1078.0</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -540,10 +894,10 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>250000.0</v>
+        <v>326800.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.002106467360178704</v>
+        <v>0.003454083376386986</v>
       </c>
     </row>
     <row r="8">
@@ -551,7 +905,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>126.0</v>
+        <v>706.0</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -560,10 +914,10 @@
         <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>1000000.0</v>
+        <v>1.37E7</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0018745448351207951</v>
+        <v>0.0032886450231915058</v>
       </c>
     </row>
     <row r="9">
@@ -571,7 +925,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>301.0</v>
+        <v>1080.0</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -580,10 +934,10 @@
         <v>21</v>
       </c>
       <c r="E9" t="n">
-        <v>152400.0</v>
+        <v>536900.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0017812521293702251</v>
+        <v>0.003236275431947603</v>
       </c>
     </row>
     <row r="10">
@@ -591,7 +945,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>43.0</v>
+        <v>1069.0</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -600,10 +954,10 @@
         <v>23</v>
       </c>
       <c r="E10" t="n">
-        <v>2900000.0</v>
+        <v>755500.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0017065213291758592</v>
+        <v>0.0031688136979365965</v>
       </c>
     </row>
     <row r="11">
@@ -623,7 +977,7 @@
         <v>1700000.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0016055906384682846</v>
+        <v>0.0031666878271890946</v>
       </c>
     </row>
     <row r="12">
@@ -631,7 +985,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>8.0</v>
+        <v>1111.0</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -640,10 +994,10 @@
         <v>27</v>
       </c>
       <c r="E12" t="n">
-        <v>980000.0</v>
+        <v>940500.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.001602099860684238</v>
+        <v>0.0031602573986769704</v>
       </c>
     </row>
     <row r="13">
@@ -651,7 +1005,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>158.0</v>
+        <v>1081.0</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -660,10 +1014,10 @@
         <v>29</v>
       </c>
       <c r="E13" t="n">
-        <v>203900.0</v>
+        <v>479000.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0012702872049738035</v>
+        <v>0.0030205572959240896</v>
       </c>
     </row>
     <row r="14">
@@ -671,7 +1025,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>337.0</v>
+        <v>805.0</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -680,10 +1034,10 @@
         <v>31</v>
       </c>
       <c r="E14" t="n">
-        <v>305300.0</v>
+        <v>2600000.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0012159757274048902</v>
+        <v>0.002923174227967788</v>
       </c>
     </row>
     <row r="15">
@@ -691,7 +1045,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>767.0</v>
+        <v>1136.0</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -700,10 +1054,10 @@
         <v>33</v>
       </c>
       <c r="E15" t="n">
-        <v>190200.0</v>
+        <v>705900.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.001162112735152395</v>
+        <v>0.002830531276523769</v>
       </c>
     </row>
     <row r="16">
@@ -711,7 +1065,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>694.0</v>
+        <v>301.0</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -720,10 +1074,10 @@
         <v>35</v>
       </c>
       <c r="E16" t="n">
-        <v>641600.0</v>
+        <v>152400.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0011587061336496673</v>
+        <v>0.002631892765690951</v>
       </c>
     </row>
     <row r="17">
@@ -731,7 +1085,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>197.0</v>
+        <v>8.0</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -740,10 +1094,10 @@
         <v>37</v>
       </c>
       <c r="E17" t="n">
-        <v>128300.0</v>
+        <v>980000.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0010410562081836008</v>
+        <v>0.002583153186769793</v>
       </c>
     </row>
     <row r="18">
@@ -751,7 +1105,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="n">
-        <v>11.0</v>
+        <v>1089.0</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -760,10 +1114,10 @@
         <v>39</v>
       </c>
       <c r="E18" t="n">
-        <v>2500000.0</v>
+        <v>487700.0</v>
       </c>
       <c r="F18" t="n">
-        <v>9.641814546719973E-4</v>
+        <v>0.002562159239731564</v>
       </c>
     </row>
     <row r="19">
@@ -771,7 +1125,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>104.0</v>
+        <v>42.0</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -780,10 +1134,10 @@
         <v>41</v>
       </c>
       <c r="E19" t="n">
-        <v>166400.0</v>
+        <v>489700.0</v>
       </c>
       <c r="F19" t="n">
-        <v>9.204181450442162E-4</v>
+        <v>0.002547655235343991</v>
       </c>
     </row>
     <row r="20">
@@ -791,7 +1145,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>831.0</v>
+        <v>1077.0</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
@@ -800,10 +1154,10 @@
         <v>43</v>
       </c>
       <c r="E20" t="n">
-        <v>4600000.0</v>
+        <v>173200.0</v>
       </c>
       <c r="F20" t="n">
-        <v>8.880367157504156E-4</v>
+        <v>0.0025217341486425977</v>
       </c>
     </row>
     <row r="21">
@@ -811,7 +1165,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>47.0</v>
+        <v>1083.0</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -820,10 +1174,10 @@
         <v>45</v>
       </c>
       <c r="E21" t="n">
-        <v>1300000.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F21" t="n">
-        <v>8.50171432300735E-4</v>
+        <v>0.0023983934729238893</v>
       </c>
     </row>
     <row r="22">
@@ -831,7 +1185,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>237.0</v>
+        <v>10.0</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -840,10 +1194,10 @@
         <v>47</v>
       </c>
       <c r="E22" t="n">
-        <v>373100.0</v>
+        <v>3400000.0</v>
       </c>
       <c r="F22" t="n">
-        <v>8.084657896825843E-4</v>
+        <v>0.0023913915030515944</v>
       </c>
     </row>
     <row r="23">
@@ -851,7 +1205,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>151.0</v>
+        <v>1125.0</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
@@ -860,10 +1214,10 @@
         <v>49</v>
       </c>
       <c r="E23" t="n">
-        <v>200300.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F23" t="n">
-        <v>7.696139291408254E-4</v>
+        <v>0.0023894571299283855</v>
       </c>
     </row>
     <row r="24">
@@ -871,7 +1225,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>241.0</v>
+        <v>1108.0</v>
       </c>
       <c r="C24" t="s">
         <v>50</v>
@@ -880,10 +1234,10 @@
         <v>51</v>
       </c>
       <c r="E24" t="n">
-        <v>397600.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="F24" t="n">
-        <v>6.287895094061276E-4</v>
+        <v>0.002357234148109494</v>
       </c>
     </row>
     <row r="25">
@@ -891,7 +1245,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>983.0</v>
+        <v>1166.0</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -900,10 +1254,10 @@
         <v>53</v>
       </c>
       <c r="E25" t="n">
-        <v>3900000.0</v>
+        <v>331500.0</v>
       </c>
       <c r="F25" t="n">
-        <v>6.155688171511946E-4</v>
+        <v>0.00232867452314156</v>
       </c>
     </row>
     <row r="26">
@@ -911,7 +1265,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>42.0</v>
+        <v>1063.0</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -920,10 +1274,10 @@
         <v>55</v>
       </c>
       <c r="E26" t="n">
-        <v>489700.0</v>
+        <v>9100000.0</v>
       </c>
       <c r="F26" t="n">
-        <v>5.908519378299151E-4</v>
+        <v>0.0023072536295465377</v>
       </c>
     </row>
     <row r="27">
@@ -931,7 +1285,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>188.0</v>
+        <v>1091.0</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -940,10 +1294,10 @@
         <v>57</v>
       </c>
       <c r="E27" t="n">
-        <v>178400.0</v>
+        <v>1600000.0</v>
       </c>
       <c r="F27" t="n">
-        <v>5.713565081479741E-4</v>
+        <v>0.0021892676297163836</v>
       </c>
     </row>
     <row r="28">
@@ -951,7 +1305,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>201.0</v>
+        <v>1223.0</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
@@ -960,10 +1314,10 @@
         <v>59</v>
       </c>
       <c r="E28" t="n">
-        <v>953900.0</v>
+        <v>1600000.0</v>
       </c>
       <c r="F28" t="n">
-        <v>5.647367792702757E-4</v>
+        <v>0.0021761907607646992</v>
       </c>
     </row>
     <row r="29">
@@ -971,7 +1325,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>521.0</v>
+        <v>126.0</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -980,10 +1334,10 @@
         <v>61</v>
       </c>
       <c r="E29" t="n">
-        <v>113400.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="F29" t="n">
-        <v>5.422097627379417E-4</v>
+        <v>0.0020922371417226096</v>
       </c>
     </row>
     <row r="30">
@@ -991,7 +1345,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>3.0</v>
+        <v>1150.0</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -1000,10 +1354,10 @@
         <v>63</v>
       </c>
       <c r="E30" t="n">
-        <v>155900.0</v>
+        <v>666500.0</v>
       </c>
       <c r="F30" t="n">
-        <v>5.422072850861932E-4</v>
+        <v>0.0020478373565942995</v>
       </c>
     </row>
     <row r="31">
@@ -1011,7 +1365,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>361.0</v>
+        <v>1219.0</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -1020,10 +1374,10 @@
         <v>65</v>
       </c>
       <c r="E31" t="n">
-        <v>148300.0</v>
+        <v>137100.0</v>
       </c>
       <c r="F31" t="n">
-        <v>4.884000502152278E-4</v>
+        <v>0.00204782398151371</v>
       </c>
     </row>
     <row r="32">
@@ -1031,7 +1385,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="n">
-        <v>302.0</v>
+        <v>1250.0</v>
       </c>
       <c r="C32" t="s">
         <v>66</v>
@@ -1040,10 +1394,10 @@
         <v>67</v>
       </c>
       <c r="E32" t="n">
-        <v>198000.0</v>
+        <v>526600.0</v>
       </c>
       <c r="F32" t="n">
-        <v>4.882455653622423E-4</v>
+        <v>0.002005362639966847</v>
       </c>
     </row>
     <row r="33">
@@ -1051,7 +1405,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="n">
-        <v>835.0</v>
+        <v>1146.0</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
@@ -1060,10 +1414,10 @@
         <v>69</v>
       </c>
       <c r="E33" t="n">
-        <v>5400000.0</v>
+        <v>3700000.0</v>
       </c>
       <c r="F33" t="n">
-        <v>4.7891095838715944E-4</v>
+        <v>0.00197836415246657</v>
       </c>
     </row>
     <row r="34">
@@ -1071,7 +1425,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="n">
-        <v>805.0</v>
+        <v>1224.0</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
@@ -1080,10 +1434,10 @@
         <v>71</v>
       </c>
       <c r="E34" t="n">
-        <v>2600000.0</v>
+        <v>3500000.0</v>
       </c>
       <c r="F34" t="n">
-        <v>4.634324173480345E-4</v>
+        <v>0.001967025861756598</v>
       </c>
     </row>
     <row r="35">
@@ -1091,7 +1445,7 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="n">
-        <v>91.0</v>
+        <v>1142.0</v>
       </c>
       <c r="C35" t="s">
         <v>72</v>
@@ -1100,10 +1454,10 @@
         <v>73</v>
       </c>
       <c r="E35" t="n">
-        <v>104400.0</v>
+        <v>715800.0</v>
       </c>
       <c r="F35" t="n">
-        <v>4.5826356671735586E-4</v>
+        <v>0.0019398043402548953</v>
       </c>
     </row>
     <row r="36">
@@ -1111,7 +1465,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="n">
-        <v>356.0</v>
+        <v>1149.0</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
@@ -1120,10 +1474,10 @@
         <v>75</v>
       </c>
       <c r="E36" t="n">
-        <v>245300.0</v>
+        <v>852900.0</v>
       </c>
       <c r="F36" t="n">
-        <v>4.054267010415546E-4</v>
+        <v>0.0018713066127666834</v>
       </c>
     </row>
     <row r="37">
@@ -1131,7 +1485,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="n">
-        <v>428.0</v>
+        <v>1182.0</v>
       </c>
       <c r="C37" t="s">
         <v>76</v>
@@ -1140,10 +1494,10 @@
         <v>77</v>
       </c>
       <c r="E37" t="n">
-        <v>310700.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="F37" t="n">
-        <v>3.75211709472828E-4</v>
+        <v>0.0018682239815331022</v>
       </c>
     </row>
     <row r="38">
@@ -1151,7 +1505,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="n">
-        <v>977.0</v>
+        <v>3.0</v>
       </c>
       <c r="C38" t="s">
         <v>78</v>
@@ -1160,10 +1514,10 @@
         <v>79</v>
       </c>
       <c r="E38" t="n">
-        <v>146300.0</v>
+        <v>155900.0</v>
       </c>
       <c r="F38" t="n">
-        <v>3.625004106454669E-4</v>
+        <v>0.001845741472303051</v>
       </c>
     </row>
     <row r="39">
@@ -1171,7 +1525,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="n">
-        <v>806.0</v>
+        <v>1097.0</v>
       </c>
       <c r="C39" t="s">
         <v>80</v>
@@ -1180,10 +1534,10 @@
         <v>81</v>
       </c>
       <c r="E39" t="n">
-        <v>140900.0</v>
+        <v>1.04E7</v>
       </c>
       <c r="F39" t="n">
-        <v>3.5252471213989187E-4</v>
+        <v>0.0018328266297893555</v>
       </c>
     </row>
     <row r="40">
@@ -1191,7 +1545,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="n">
-        <v>20.0</v>
+        <v>1211.0</v>
       </c>
       <c r="C40" t="s">
         <v>82</v>
@@ -1200,10 +1554,10 @@
         <v>83</v>
       </c>
       <c r="E40" t="n">
-        <v>260500.0</v>
+        <v>100400.0</v>
       </c>
       <c r="F40" t="n">
-        <v>3.416766250410644E-4</v>
+        <v>0.0017396214595074323</v>
       </c>
     </row>
     <row r="41">
@@ -1211,7 +1565,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="n">
-        <v>845.0</v>
+        <v>20.0</v>
       </c>
       <c r="C41" t="s">
         <v>84</v>
@@ -1220,10 +1574,10 @@
         <v>85</v>
       </c>
       <c r="E41" t="n">
-        <v>1100000.0</v>
+        <v>260500.0</v>
       </c>
       <c r="F41" t="n">
-        <v>3.340521190990837E-4</v>
+        <v>0.0017317124341041331</v>
       </c>
     </row>
     <row r="42">
@@ -1231,7 +1585,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="n">
-        <v>440.0</v>
+        <v>1084.0</v>
       </c>
       <c r="C42" t="s">
         <v>86</v>
@@ -1240,10 +1594,10 @@
         <v>87</v>
       </c>
       <c r="E42" t="n">
-        <v>702500.0</v>
+        <v>2100000.0</v>
       </c>
       <c r="F42" t="n">
-        <v>3.324592949494473E-4</v>
+        <v>0.0017266867534972193</v>
       </c>
     </row>
     <row r="43">
@@ -1251,7 +1605,7 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="n">
-        <v>103.0</v>
+        <v>1070.0</v>
       </c>
       <c r="C43" t="s">
         <v>88</v>
@@ -1260,10 +1614,10 @@
         <v>89</v>
       </c>
       <c r="E43" t="n">
-        <v>1000000.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F43" t="n">
-        <v>3.241180571394148E-4</v>
+        <v>0.0016572922303062722</v>
       </c>
     </row>
     <row r="44">
@@ -1271,7 +1625,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="n">
-        <v>268.0</v>
+        <v>38.0</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
@@ -1280,10 +1634,10 @@
         <v>91</v>
       </c>
       <c r="E44" t="n">
-        <v>592100.0</v>
+        <v>154300.0</v>
       </c>
       <c r="F44" t="n">
-        <v>3.214742713130093E-4</v>
+        <v>0.001649971768858667</v>
       </c>
     </row>
     <row r="45">
@@ -1291,7 +1645,7 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="n">
-        <v>978.0</v>
+        <v>197.0</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
@@ -1300,10 +1654,10 @@
         <v>93</v>
       </c>
       <c r="E45" t="n">
-        <v>1700000.0</v>
+        <v>128300.0</v>
       </c>
       <c r="F45" t="n">
-        <v>3.196546852086947E-4</v>
+        <v>0.0016159391271390506</v>
       </c>
     </row>
     <row r="46">
@@ -1311,7 +1665,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="n">
-        <v>737.0</v>
+        <v>1214.0</v>
       </c>
       <c r="C46" t="s">
         <v>94</v>
@@ -1320,10 +1674,10 @@
         <v>95</v>
       </c>
       <c r="E46" t="n">
-        <v>231900.0</v>
+        <v>882500.0</v>
       </c>
       <c r="F46" t="n">
-        <v>3.0433642136535997E-4</v>
+        <v>0.0015939451252695532</v>
       </c>
     </row>
     <row r="47">
@@ -1331,7 +1685,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="n">
-        <v>976.0</v>
+        <v>13.0</v>
       </c>
       <c r="C47" t="s">
         <v>96</v>
@@ -1340,10 +1694,10 @@
         <v>97</v>
       </c>
       <c r="E47" t="n">
-        <v>270900.0</v>
+        <v>2800000.0</v>
       </c>
       <c r="F47" t="n">
-        <v>2.9238987854094886E-4</v>
+        <v>0.0015498902142121805</v>
       </c>
     </row>
     <row r="48">
@@ -1351,7 +1705,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="n">
-        <v>30.0</v>
+        <v>1094.0</v>
       </c>
       <c r="C48" t="s">
         <v>98</v>
@@ -1360,10 +1714,10 @@
         <v>99</v>
       </c>
       <c r="E48" t="n">
-        <v>241400.0</v>
+        <v>4300000.0</v>
       </c>
       <c r="F48" t="n">
-        <v>2.8741187152286077E-4</v>
+        <v>0.0015290868014505466</v>
       </c>
     </row>
     <row r="49">
@@ -1371,7 +1725,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="n">
-        <v>480.0</v>
+        <v>237.0</v>
       </c>
       <c r="C49" t="s">
         <v>100</v>
@@ -1380,10 +1734,10 @@
         <v>101</v>
       </c>
       <c r="E49" t="n">
-        <v>417100.0</v>
+        <v>373100.0</v>
       </c>
       <c r="F49" t="n">
-        <v>2.8265936962469814E-4</v>
+        <v>0.0015079122473889782</v>
       </c>
     </row>
     <row r="50">
@@ -1391,7 +1745,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="n">
-        <v>45.0</v>
+        <v>1200.0</v>
       </c>
       <c r="C50" t="s">
         <v>102</v>
@@ -1400,10 +1754,10 @@
         <v>103</v>
       </c>
       <c r="E50" t="n">
-        <v>543000.0</v>
+        <v>2000000.0</v>
       </c>
       <c r="F50" t="n">
-        <v>2.7823568197261477E-4</v>
+        <v>0.001484406162205089</v>
       </c>
     </row>
     <row r="51">
@@ -1411,7 +1765,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="n">
-        <v>804.0</v>
+        <v>1267.0</v>
       </c>
       <c r="C51" t="s">
         <v>104</v>
@@ -1420,10 +1774,10 @@
         <v>105</v>
       </c>
       <c r="E51" t="n">
-        <v>298000.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="F51" t="n">
-        <v>2.724638011144163E-4</v>
+        <v>0.0014720752443313071</v>
       </c>
     </row>
     <row r="52">
@@ -1431,7 +1785,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="n">
-        <v>257.0</v>
+        <v>243.0</v>
       </c>
       <c r="C52" t="s">
         <v>106</v>
@@ -1440,10 +1794,10 @@
         <v>107</v>
       </c>
       <c r="E52" t="n">
-        <v>509800.0</v>
+        <v>250000.0</v>
       </c>
       <c r="F52" t="n">
-        <v>2.7180861295567744E-4</v>
+        <v>0.0014711010805139924</v>
       </c>
     </row>
     <row r="53">
@@ -1451,7 +1805,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="n">
-        <v>495.0</v>
+        <v>1151.0</v>
       </c>
       <c r="C53" t="s">
         <v>108</v>
@@ -1460,10 +1814,10 @@
         <v>109</v>
       </c>
       <c r="E53" t="n">
-        <v>568300.0</v>
+        <v>241400.0</v>
       </c>
       <c r="F53" t="n">
-        <v>2.694482723252261E-4</v>
+        <v>0.0014250279011344855</v>
       </c>
     </row>
     <row r="54">
@@ -1471,7 +1825,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="n">
-        <v>72.0</v>
+        <v>1373.0</v>
       </c>
       <c r="C54" t="s">
         <v>110</v>
@@ -1480,10 +1834,1190 @@
         <v>111</v>
       </c>
       <c r="E54" t="n">
+        <v>224500.0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.0014038033062826775</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1103.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55" t="n">
+        <v>481900.0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.001394603436555941</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1131.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" t="n">
+        <v>171000.0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.0013759937276162449</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1118.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" t="n">
+        <v>157100.0</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.0013294576989969016</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1088.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" t="n">
+        <v>404200.0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0013125929690690438</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1071.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>120</v>
+      </c>
+      <c r="D59" t="s">
+        <v>121</v>
+      </c>
+      <c r="E59" t="n">
+        <v>6200000.0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.0012959398567290465</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="n">
+        <v>857.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3600000.0</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.001273933286680056</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D61" t="s">
+        <v>125</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1300000.0</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.001271553545097293</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1287.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>126</v>
+      </c>
+      <c r="D62" t="s">
+        <v>127</v>
+      </c>
+      <c r="E62" t="n">
+        <v>163500.0</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.0012366779115893678</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B63" t="n">
+        <v>337.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>128</v>
+      </c>
+      <c r="D63" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" t="n">
+        <v>305300.0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0012311235597134169</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" t="s">
+        <v>131</v>
+      </c>
+      <c r="E64" t="n">
+        <v>166400.0</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0012112632492142861</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1222.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" t="s">
+        <v>133</v>
+      </c>
+      <c r="E65" t="n">
+        <v>6700000.0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.00116957435239394</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B66" t="n">
+        <v>356.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" t="n">
+        <v>245300.0</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.0011688447110106389</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B67" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" t="n">
+        <v>203900.0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.0011616585102903483</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1207.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" t="s">
+        <v>139</v>
+      </c>
+      <c r="E68" t="n">
+        <v>787700.0</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.001155870420949607</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="B69" t="n">
+        <v>831.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D69" t="s">
+        <v>141</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4600000.0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.0011111016606237564</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B70" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2900000.0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.0010976534961880764</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1127.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>144</v>
+      </c>
+      <c r="D71" t="s">
+        <v>145</v>
+      </c>
+      <c r="E71" t="n">
+        <v>126300.0</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.0010610562832355363</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1143.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>146</v>
+      </c>
+      <c r="D72" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" t="n">
+        <v>292300.0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.001028630144684395</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1215.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>148</v>
+      </c>
+      <c r="D73" t="s">
+        <v>149</v>
+      </c>
+      <c r="E73" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.001025420314069198</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1345.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>150</v>
+      </c>
+      <c r="D74" t="s">
+        <v>151</v>
+      </c>
+      <c r="E74" t="n">
+        <v>339700.0</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.0010169073878611857</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1170.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>152</v>
+      </c>
+      <c r="D75" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" t="n">
+        <v>184500.0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.0010151182938364098</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="B76" t="n">
+        <v>835.0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>154</v>
+      </c>
+      <c r="D76" t="s">
+        <v>155</v>
+      </c>
+      <c r="E76" t="n">
+        <v>5400000.0</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.0010123507282164348</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="B77" t="n">
+        <v>257.0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" t="s">
+        <v>157</v>
+      </c>
+      <c r="E77" t="n">
+        <v>509800.0</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.0010049548016196304</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="B78" t="n">
+        <v>977.0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" t="n">
+        <v>146300.0</v>
+      </c>
+      <c r="F78" t="n">
+        <v>9.78212794825438E-4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1227.0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>160</v>
+      </c>
+      <c r="D79" t="s">
+        <v>161</v>
+      </c>
+      <c r="E79" t="n">
+        <v>2600000.0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>8.27381367591047E-4</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1188.0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>162</v>
+      </c>
+      <c r="D80" t="s">
+        <v>163</v>
+      </c>
+      <c r="E80" t="n">
+        <v>167300.0</v>
+      </c>
+      <c r="F80" t="n">
+        <v>7.373326331429075E-4</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="B81" t="n">
+        <v>1375.0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" t="s">
+        <v>165</v>
+      </c>
+      <c r="E81" t="n">
+        <v>655400.0</v>
+      </c>
+      <c r="F81" t="n">
+        <v>7.096055591669049E-4</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1370.0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>166</v>
+      </c>
+      <c r="D82" t="s">
+        <v>167</v>
+      </c>
+      <c r="E82" t="n">
+        <v>879400.0</v>
+      </c>
+      <c r="F82" t="n">
+        <v>6.524213440969598E-4</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="B83" t="n">
+        <v>480.0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>168</v>
+      </c>
+      <c r="D83" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" t="n">
+        <v>417100.0</v>
+      </c>
+      <c r="F83" t="n">
+        <v>6.40408297274015E-4</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="B84" t="n">
+        <v>521.0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>170</v>
+      </c>
+      <c r="D84" t="s">
+        <v>171</v>
+      </c>
+      <c r="E84" t="n">
+        <v>113400.0</v>
+      </c>
+      <c r="F84" t="n">
+        <v>6.301651643602331E-4</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="B85" t="n">
+        <v>983.0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>172</v>
+      </c>
+      <c r="D85" t="s">
+        <v>173</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3900000.0</v>
+      </c>
+      <c r="F85" t="n">
+        <v>6.25313599423853E-4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="B86" t="n">
+        <v>495.0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>174</v>
+      </c>
+      <c r="D86" t="s">
+        <v>175</v>
+      </c>
+      <c r="E86" t="n">
+        <v>568300.0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>6.22784459467402E-4</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="B87" t="n">
+        <v>201.0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>176</v>
+      </c>
+      <c r="D87" t="s">
+        <v>177</v>
+      </c>
+      <c r="E87" t="n">
+        <v>953900.0</v>
+      </c>
+      <c r="F87" t="n">
+        <v>6.195029947111693E-4</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="B88" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>178</v>
+      </c>
+      <c r="D88" t="s">
+        <v>179</v>
+      </c>
+      <c r="E88" t="n">
+        <v>641600.0</v>
+      </c>
+      <c r="F88" t="n">
+        <v>6.171484291588259E-4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="B89" t="n">
+        <v>188.0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>180</v>
+      </c>
+      <c r="D89" t="s">
+        <v>181</v>
+      </c>
+      <c r="E89" t="n">
+        <v>178400.0</v>
+      </c>
+      <c r="F89" t="n">
+        <v>5.927414956636031E-4</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="B90" t="n">
+        <v>1265.0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>182</v>
+      </c>
+      <c r="D90" t="s">
+        <v>183</v>
+      </c>
+      <c r="E90" t="n">
+        <v>344700.0</v>
+      </c>
+      <c r="F90" t="n">
+        <v>5.881287769164997E-4</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="B91" t="n">
+        <v>767.0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>184</v>
+      </c>
+      <c r="D91" t="s">
+        <v>185</v>
+      </c>
+      <c r="E91" t="n">
+        <v>190200.0</v>
+      </c>
+      <c r="F91" t="n">
+        <v>5.616130141445785E-4</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="B92" t="n">
+        <v>1329.0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>186</v>
+      </c>
+      <c r="D92" t="s">
+        <v>187</v>
+      </c>
+      <c r="E92" t="n">
+        <v>345400.0</v>
+      </c>
+      <c r="F92" t="n">
+        <v>5.383338208003807E-4</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1369.0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>188</v>
+      </c>
+      <c r="D93" t="s">
+        <v>189</v>
+      </c>
+      <c r="E93" t="n">
+        <v>3200000.0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>5.352959104816847E-4</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="B94" t="n">
+        <v>241.0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>190</v>
+      </c>
+      <c r="D94" t="s">
+        <v>191</v>
+      </c>
+      <c r="E94" t="n">
+        <v>397600.0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>4.39129959566401E-4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="B95" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>192</v>
+      </c>
+      <c r="D95" t="s">
+        <v>193</v>
+      </c>
+      <c r="E95" t="n">
+        <v>104400.0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>3.994175207385139E-4</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="B96" t="n">
+        <v>268.0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>194</v>
+      </c>
+      <c r="D96" t="s">
+        <v>195</v>
+      </c>
+      <c r="E96" t="n">
+        <v>592100.0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>3.841850010579132E-4</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="B97" t="n">
+        <v>804.0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>196</v>
+      </c>
+      <c r="D97" t="s">
+        <v>197</v>
+      </c>
+      <c r="E97" t="n">
+        <v>298000.0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>3.6793304517648335E-4</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="B98" t="n">
+        <v>806.0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" t="s">
+        <v>199</v>
+      </c>
+      <c r="E98" t="n">
+        <v>140900.0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>3.505225356584713E-4</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="B99" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>200</v>
+      </c>
+      <c r="D99" t="s">
+        <v>201</v>
+      </c>
+      <c r="E99" t="n">
+        <v>241400.0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>3.411643748846318E-4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="B100" t="n">
+        <v>361.0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>202</v>
+      </c>
+      <c r="D100" t="s">
+        <v>203</v>
+      </c>
+      <c r="E100" t="n">
+        <v>148300.0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>3.4108567508672744E-4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="B101" t="n">
+        <v>302.0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>204</v>
+      </c>
+      <c r="D101" t="s">
+        <v>205</v>
+      </c>
+      <c r="E101" t="n">
+        <v>198000.0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>3.2856659471996015E-4</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B102" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>206</v>
+      </c>
+      <c r="D102" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" t="n">
+        <v>543000.0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>3.2823604260689336E-4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B103" t="n">
+        <v>1332.0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>208</v>
+      </c>
+      <c r="D103" t="s">
+        <v>209</v>
+      </c>
+      <c r="E103" t="n">
+        <v>2900000.0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>3.2649487653549765E-4</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B104" t="n">
+        <v>1317.0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>210</v>
+      </c>
+      <c r="D104" t="s">
+        <v>211</v>
+      </c>
+      <c r="E104" t="n">
+        <v>818600.0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>3.1724561867124457E-4</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="B105" t="n">
+        <v>737.0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>212</v>
+      </c>
+      <c r="D105" t="s">
+        <v>213</v>
+      </c>
+      <c r="E105" t="n">
+        <v>231900.0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>2.927223951709339E-4</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="B106" t="n">
+        <v>428.0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>214</v>
+      </c>
+      <c r="D106" t="s">
+        <v>215</v>
+      </c>
+      <c r="E106" t="n">
+        <v>310700.0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>2.613301180496958E-4</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="B107" t="n">
+        <v>845.0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>216</v>
+      </c>
+      <c r="D107" t="s">
+        <v>217</v>
+      </c>
+      <c r="E107" t="n">
+        <v>1100000.0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>2.332931630675543E-4</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="B108" t="n">
+        <v>440.0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>218</v>
+      </c>
+      <c r="D108" t="s">
+        <v>219</v>
+      </c>
+      <c r="E108" t="n">
+        <v>702500.0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>2.3218077681752474E-4</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="B109" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>220</v>
+      </c>
+      <c r="D109" t="s">
+        <v>221</v>
+      </c>
+      <c r="E109" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>2.2752300685140197E-4</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="B110" t="n">
+        <v>978.0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>222</v>
+      </c>
+      <c r="D110" t="s">
+        <v>223</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1700000.0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>2.2323837610376142E-4</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="B111" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>224</v>
+      </c>
+      <c r="D111" t="s">
+        <v>225</v>
+      </c>
+      <c r="E111" t="n">
+        <v>200300.0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>2.1420205286809102E-4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="B112" t="n">
+        <v>976.0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>226</v>
+      </c>
+      <c r="D112" t="s">
+        <v>227</v>
+      </c>
+      <c r="E112" t="n">
+        <v>270900.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>2.0419735638175476E-4</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="B113" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>228</v>
+      </c>
+      <c r="D113" t="s">
+        <v>229</v>
+      </c>
+      <c r="E113" t="n">
         <v>186300.0</v>
       </c>
-      <c r="F54" t="n">
-        <v>2.559377602173589E-4</v>
+      <c r="F113" t="n">
+        <v>1.7874016123760222E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KoL is more useful now
</commit_message>
<xml_diff>
--- a/twitter-influencer-ranking/ranking_output.xlsx
+++ b/twitter-influencer-ranking/ranking_output.xlsx
@@ -797,7 +797,7 @@
         <v>2.067E8</v>
       </c>
       <c r="F2" t="n">
-        <v>0.004783248567557784</v>
+        <v>0.004783248567557789</v>
       </c>
     </row>
     <row r="3">
@@ -817,7 +817,7 @@
         <v>2300000.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004693870929501009</v>
+        <v>0.004693870929501013</v>
       </c>
     </row>
     <row r="4">
@@ -837,7 +837,7 @@
         <v>2900000.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.004366238061226845</v>
+        <v>0.004366238061226849</v>
       </c>
     </row>
     <row r="5">
@@ -857,7 +857,7 @@
         <v>292300.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004274227260107351</v>
+        <v>0.004274227260107357</v>
       </c>
     </row>
     <row r="6">
@@ -877,7 +877,7 @@
         <v>2500000.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00353142275637502</v>
+        <v>0.003531422756375024</v>
       </c>
     </row>
     <row r="7">
@@ -897,7 +897,7 @@
         <v>326800.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.003454083376386986</v>
+        <v>0.0034540833763869886</v>
       </c>
     </row>
     <row r="8">
@@ -917,7 +917,7 @@
         <v>1.37E7</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0032886450231915058</v>
+        <v>0.0032886450231915084</v>
       </c>
     </row>
     <row r="9">
@@ -937,7 +937,7 @@
         <v>536900.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.003236275431947603</v>
+        <v>0.0032362754319476064</v>
       </c>
     </row>
     <row r="10">
@@ -957,7 +957,7 @@
         <v>755500.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0031688136979365965</v>
+        <v>0.0031688136979366004</v>
       </c>
     </row>
     <row r="11">
@@ -977,7 +977,7 @@
         <v>1700000.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0031666878271890946</v>
+        <v>0.0031666878271890977</v>
       </c>
     </row>
     <row r="12">
@@ -997,7 +997,7 @@
         <v>940500.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0031602573986769704</v>
+        <v>0.003160257398676974</v>
       </c>
     </row>
     <row r="13">
@@ -1017,7 +1017,7 @@
         <v>479000.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0030205572959240896</v>
+        <v>0.003020557295924092</v>
       </c>
     </row>
     <row r="14">
@@ -1037,7 +1037,7 @@
         <v>2600000.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.002923174227967788</v>
+        <v>0.00292317422796779</v>
       </c>
     </row>
     <row r="15">
@@ -1057,7 +1057,7 @@
         <v>705900.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.002830531276523769</v>
+        <v>0.0028305312765237707</v>
       </c>
     </row>
     <row r="16">
@@ -1077,7 +1077,7 @@
         <v>152400.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.002631892765690951</v>
+        <v>0.0026318927656909527</v>
       </c>
     </row>
     <row r="17">
@@ -1097,7 +1097,7 @@
         <v>980000.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.002583153186769793</v>
+        <v>0.0025831531867697953</v>
       </c>
     </row>
     <row r="18">
@@ -1117,7 +1117,7 @@
         <v>487700.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.002562159239731564</v>
+        <v>0.002562159239731566</v>
       </c>
     </row>
     <row r="19">
@@ -1137,7 +1137,7 @@
         <v>489700.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.002547655235343991</v>
+        <v>0.0025476552353439932</v>
       </c>
     </row>
     <row r="20">
@@ -1157,7 +1157,7 @@
         <v>173200.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0025217341486425977</v>
+        <v>0.002521734148642599</v>
       </c>
     </row>
     <row r="21">
@@ -1177,7 +1177,7 @@
         <v>1400000.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0023983934729238893</v>
+        <v>0.0023983934729238914</v>
       </c>
     </row>
     <row r="22">
@@ -1197,7 +1197,7 @@
         <v>3400000.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0023913915030515944</v>
+        <v>0.002391391503051597</v>
       </c>
     </row>
     <row r="23">
@@ -1217,7 +1217,7 @@
         <v>1400000.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0023894571299283855</v>
+        <v>0.0023894571299283877</v>
       </c>
     </row>
     <row r="24">
@@ -1237,7 +1237,7 @@
         <v>1500000.0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.002357234148109494</v>
+        <v>0.0023572341481094953</v>
       </c>
     </row>
     <row r="25">
@@ -1257,7 +1257,7 @@
         <v>331500.0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.00232867452314156</v>
+        <v>0.0023286745231415624</v>
       </c>
     </row>
     <row r="26">
@@ -1277,7 +1277,7 @@
         <v>9100000.0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0023072536295465377</v>
+        <v>0.00230725362954654</v>
       </c>
     </row>
     <row r="27">
@@ -1297,7 +1297,7 @@
         <v>1600000.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0021892676297163836</v>
+        <v>0.0021892676297163858</v>
       </c>
     </row>
     <row r="28">
@@ -1317,7 +1317,7 @@
         <v>1600000.0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0021761907607646992</v>
+        <v>0.002176190760764701</v>
       </c>
     </row>
     <row r="29">
@@ -1337,7 +1337,7 @@
         <v>1000000.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0020922371417226096</v>
+        <v>0.002092237141722611</v>
       </c>
     </row>
     <row r="30">
@@ -1357,7 +1357,7 @@
         <v>666500.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0020478373565942995</v>
+        <v>0.002047837356594302</v>
       </c>
     </row>
     <row r="31">
@@ -1377,7 +1377,7 @@
         <v>137100.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.00204782398151371</v>
+        <v>0.002047823981513712</v>
       </c>
     </row>
     <row r="32">
@@ -1397,7 +1397,7 @@
         <v>526600.0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.002005362639966847</v>
+        <v>0.0020053626399668487</v>
       </c>
     </row>
     <row r="33">
@@ -1417,7 +1417,7 @@
         <v>3700000.0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00197836415246657</v>
+        <v>0.0019783641524665713</v>
       </c>
     </row>
     <row r="34">
@@ -1437,7 +1437,7 @@
         <v>3500000.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.001967025861756598</v>
+        <v>0.0019670258617565995</v>
       </c>
     </row>
     <row r="35">
@@ -1457,7 +1457,7 @@
         <v>715800.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0019398043402548953</v>
+        <v>0.0019398043402548972</v>
       </c>
     </row>
     <row r="36">
@@ -1477,7 +1477,7 @@
         <v>852900.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.0018713066127666834</v>
+        <v>0.0018713066127666847</v>
       </c>
     </row>
     <row r="37">
@@ -1497,7 +1497,7 @@
         <v>1100000.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0018682239815331022</v>
+        <v>0.0018682239815331035</v>
       </c>
     </row>
     <row r="38">
@@ -1517,7 +1517,7 @@
         <v>155900.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.001845741472303051</v>
+        <v>0.0018457414723030525</v>
       </c>
     </row>
     <row r="39">
@@ -1537,7 +1537,7 @@
         <v>1.04E7</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0018328266297893555</v>
+        <v>0.001832826629789357</v>
       </c>
     </row>
     <row r="40">
@@ -1557,7 +1557,7 @@
         <v>100400.0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0017396214595074323</v>
+        <v>0.001739621459507434</v>
       </c>
     </row>
     <row r="41">
@@ -1577,7 +1577,7 @@
         <v>260500.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0017317124341041331</v>
+        <v>0.0017317124341041344</v>
       </c>
     </row>
     <row r="42">
@@ -1597,7 +1597,7 @@
         <v>2100000.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0017266867534972193</v>
+        <v>0.0017266867534972208</v>
       </c>
     </row>
     <row r="43">
@@ -1617,7 +1617,7 @@
         <v>1400000.0</v>
       </c>
       <c r="F43" t="n">
-        <v>0.0016572922303062722</v>
+        <v>0.0016572922303062735</v>
       </c>
     </row>
     <row r="44">
@@ -1637,7 +1637,7 @@
         <v>154300.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.001649971768858667</v>
+        <v>0.001649971768858668</v>
       </c>
     </row>
     <row r="45">
@@ -1657,7 +1657,7 @@
         <v>128300.0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.0016159391271390506</v>
+        <v>0.001615939127139052</v>
       </c>
     </row>
     <row r="46">
@@ -1677,7 +1677,7 @@
         <v>882500.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0015939451252695532</v>
+        <v>0.0015939451252695545</v>
       </c>
     </row>
     <row r="47">
@@ -1697,7 +1697,7 @@
         <v>2800000.0</v>
       </c>
       <c r="F47" t="n">
-        <v>0.0015498902142121805</v>
+        <v>0.001549890214212182</v>
       </c>
     </row>
     <row r="48">
@@ -1717,7 +1717,7 @@
         <v>4300000.0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0015290868014505466</v>
+        <v>0.001529086801450548</v>
       </c>
     </row>
     <row r="49">
@@ -1737,7 +1737,7 @@
         <v>373100.0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0015079122473889782</v>
+        <v>0.0015079122473889797</v>
       </c>
     </row>
     <row r="50">
@@ -1757,7 +1757,7 @@
         <v>2000000.0</v>
       </c>
       <c r="F50" t="n">
-        <v>0.001484406162205089</v>
+        <v>0.0014844061622050903</v>
       </c>
     </row>
     <row r="51">
@@ -1777,7 +1777,7 @@
         <v>1100000.0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0014720752443313071</v>
+        <v>0.0014720752443313084</v>
       </c>
     </row>
     <row r="52">
@@ -1797,7 +1797,7 @@
         <v>250000.0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.0014711010805139924</v>
+        <v>0.0014711010805139937</v>
       </c>
     </row>
     <row r="53">
@@ -1817,7 +1817,7 @@
         <v>241400.0</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0014250279011344855</v>
+        <v>0.0014250279011344864</v>
       </c>
     </row>
     <row r="54">
@@ -1837,7 +1837,7 @@
         <v>224500.0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0014038033062826775</v>
+        <v>0.0014038033062826786</v>
       </c>
     </row>
     <row r="55">
@@ -1857,7 +1857,7 @@
         <v>481900.0</v>
       </c>
       <c r="F55" t="n">
-        <v>0.001394603436555941</v>
+        <v>0.0013946034365559423</v>
       </c>
     </row>
     <row r="56">
@@ -1877,7 +1877,7 @@
         <v>171000.0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0013759937276162449</v>
+        <v>0.001375993727616246</v>
       </c>
     </row>
     <row r="57">
@@ -1897,7 +1897,7 @@
         <v>157100.0</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0013294576989969016</v>
+        <v>0.0013294576989969027</v>
       </c>
     </row>
     <row r="58">
@@ -1917,7 +1917,7 @@
         <v>404200.0</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0013125929690690438</v>
+        <v>0.0013125929690690446</v>
       </c>
     </row>
     <row r="59">
@@ -1937,7 +1937,7 @@
         <v>6200000.0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0012959398567290465</v>
+        <v>0.0012959398567290482</v>
       </c>
     </row>
     <row r="60">
@@ -1957,7 +1957,7 @@
         <v>3600000.0</v>
       </c>
       <c r="F60" t="n">
-        <v>0.001273933286680056</v>
+        <v>0.0012739332866800574</v>
       </c>
     </row>
     <row r="61">
@@ -1977,7 +1977,7 @@
         <v>1300000.0</v>
       </c>
       <c r="F61" t="n">
-        <v>0.001271553545097293</v>
+        <v>0.0012715535450972936</v>
       </c>
     </row>
     <row r="62">
@@ -1997,7 +1997,7 @@
         <v>163500.0</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0012366779115893678</v>
+        <v>0.001236677911589369</v>
       </c>
     </row>
     <row r="63">
@@ -2017,7 +2017,7 @@
         <v>305300.0</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0012311235597134169</v>
+        <v>0.0012311235597134177</v>
       </c>
     </row>
     <row r="64">
@@ -2037,7 +2037,7 @@
         <v>166400.0</v>
       </c>
       <c r="F64" t="n">
-        <v>0.0012112632492142861</v>
+        <v>0.0012112632492142868</v>
       </c>
     </row>
     <row r="65">
@@ -2057,7 +2057,7 @@
         <v>6700000.0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.00116957435239394</v>
+        <v>0.0011695743523939411</v>
       </c>
     </row>
     <row r="66">
@@ -2077,7 +2077,7 @@
         <v>245300.0</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0011688447110106389</v>
+        <v>0.0011688447110106397</v>
       </c>
     </row>
     <row r="67">
@@ -2097,7 +2097,7 @@
         <v>203900.0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.0011616585102903483</v>
+        <v>0.0011616585102903491</v>
       </c>
     </row>
     <row r="68">
@@ -2117,7 +2117,7 @@
         <v>787700.0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.001155870420949607</v>
+        <v>0.001155870420949608</v>
       </c>
     </row>
     <row r="69">
@@ -2137,7 +2137,7 @@
         <v>4600000.0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.0011111016606237564</v>
+        <v>0.001111101660623757</v>
       </c>
     </row>
     <row r="70">
@@ -2157,7 +2157,7 @@
         <v>2900000.0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.0010976534961880764</v>
+        <v>0.0010976534961880773</v>
       </c>
     </row>
     <row r="71">
@@ -2177,7 +2177,7 @@
         <v>126300.0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0010610562832355363</v>
+        <v>0.001061056283235537</v>
       </c>
     </row>
     <row r="72">
@@ -2197,7 +2197,7 @@
         <v>292300.0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.001028630144684395</v>
+        <v>0.001028630144684396</v>
       </c>
     </row>
     <row r="73">
@@ -2217,7 +2217,7 @@
         <v>1000000.0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.001025420314069198</v>
+        <v>0.0010254203140691986</v>
       </c>
     </row>
     <row r="74">
@@ -2237,7 +2237,7 @@
         <v>339700.0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.0010169073878611857</v>
+        <v>0.0010169073878611864</v>
       </c>
     </row>
     <row r="75">
@@ -2257,7 +2257,7 @@
         <v>184500.0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.0010151182938364098</v>
+        <v>0.0010151182938364107</v>
       </c>
     </row>
     <row r="76">
@@ -2277,7 +2277,7 @@
         <v>5400000.0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.0010123507282164348</v>
+        <v>0.0010123507282164357</v>
       </c>
     </row>
     <row r="77">
@@ -2297,7 +2297,7 @@
         <v>509800.0</v>
       </c>
       <c r="F77" t="n">
-        <v>0.0010049548016196304</v>
+        <v>0.0010049548016196313</v>
       </c>
     </row>
     <row r="78">
@@ -2317,7 +2317,7 @@
         <v>146300.0</v>
       </c>
       <c r="F78" t="n">
-        <v>9.78212794825438E-4</v>
+        <v>9.78212794825439E-4</v>
       </c>
     </row>
     <row r="79">
@@ -2337,7 +2337,7 @@
         <v>2600000.0</v>
       </c>
       <c r="F79" t="n">
-        <v>8.27381367591047E-4</v>
+        <v>8.273813675910476E-4</v>
       </c>
     </row>
     <row r="80">
@@ -2357,7 +2357,7 @@
         <v>167300.0</v>
       </c>
       <c r="F80" t="n">
-        <v>7.373326331429075E-4</v>
+        <v>7.373326331429079E-4</v>
       </c>
     </row>
     <row r="81">
@@ -2377,7 +2377,7 @@
         <v>655400.0</v>
       </c>
       <c r="F81" t="n">
-        <v>7.096055591669049E-4</v>
+        <v>7.096055591669057E-4</v>
       </c>
     </row>
     <row r="82">
@@ -2397,7 +2397,7 @@
         <v>879400.0</v>
       </c>
       <c r="F82" t="n">
-        <v>6.524213440969598E-4</v>
+        <v>6.524213440969603E-4</v>
       </c>
     </row>
     <row r="83">
@@ -2417,7 +2417,7 @@
         <v>417100.0</v>
       </c>
       <c r="F83" t="n">
-        <v>6.40408297274015E-4</v>
+        <v>6.404082972740156E-4</v>
       </c>
     </row>
     <row r="84">
@@ -2437,7 +2437,7 @@
         <v>113400.0</v>
       </c>
       <c r="F84" t="n">
-        <v>6.301651643602331E-4</v>
+        <v>6.301651643602337E-4</v>
       </c>
     </row>
     <row r="85">
@@ -2457,7 +2457,7 @@
         <v>3900000.0</v>
       </c>
       <c r="F85" t="n">
-        <v>6.25313599423853E-4</v>
+        <v>6.253135994238536E-4</v>
       </c>
     </row>
     <row r="86">
@@ -2477,7 +2477,7 @@
         <v>568300.0</v>
       </c>
       <c r="F86" t="n">
-        <v>6.22784459467402E-4</v>
+        <v>6.227844594674023E-4</v>
       </c>
     </row>
     <row r="87">
@@ -2497,7 +2497,7 @@
         <v>953900.0</v>
       </c>
       <c r="F87" t="n">
-        <v>6.195029947111693E-4</v>
+        <v>6.195029947111697E-4</v>
       </c>
     </row>
     <row r="88">
@@ -2517,7 +2517,7 @@
         <v>641600.0</v>
       </c>
       <c r="F88" t="n">
-        <v>6.171484291588259E-4</v>
+        <v>6.171484291588263E-4</v>
       </c>
     </row>
     <row r="89">
@@ -2537,7 +2537,7 @@
         <v>178400.0</v>
       </c>
       <c r="F89" t="n">
-        <v>5.927414956636031E-4</v>
+        <v>5.927414956636035E-4</v>
       </c>
     </row>
     <row r="90">
@@ -2557,7 +2557,7 @@
         <v>344700.0</v>
       </c>
       <c r="F90" t="n">
-        <v>5.881287769164997E-4</v>
+        <v>5.881287769165003E-4</v>
       </c>
     </row>
     <row r="91">
@@ -2577,7 +2577,7 @@
         <v>190200.0</v>
       </c>
       <c r="F91" t="n">
-        <v>5.616130141445785E-4</v>
+        <v>5.61613014144579E-4</v>
       </c>
     </row>
     <row r="92">
@@ -2597,7 +2597,7 @@
         <v>345400.0</v>
       </c>
       <c r="F92" t="n">
-        <v>5.383338208003807E-4</v>
+        <v>5.383338208003811E-4</v>
       </c>
     </row>
     <row r="93">
@@ -2617,7 +2617,7 @@
         <v>3200000.0</v>
       </c>
       <c r="F93" t="n">
-        <v>5.352959104816847E-4</v>
+        <v>5.352959104816851E-4</v>
       </c>
     </row>
     <row r="94">
@@ -2637,7 +2637,7 @@
         <v>397600.0</v>
       </c>
       <c r="F94" t="n">
-        <v>4.39129959566401E-4</v>
+        <v>4.3912995956640134E-4</v>
       </c>
     </row>
     <row r="95">
@@ -2657,7 +2657,7 @@
         <v>104400.0</v>
       </c>
       <c r="F95" t="n">
-        <v>3.994175207385139E-4</v>
+        <v>3.9941752073851427E-4</v>
       </c>
     </row>
     <row r="96">
@@ -2677,7 +2677,7 @@
         <v>592100.0</v>
       </c>
       <c r="F96" t="n">
-        <v>3.841850010579132E-4</v>
+        <v>3.841850010579135E-4</v>
       </c>
     </row>
     <row r="97">
@@ -2697,7 +2697,7 @@
         <v>298000.0</v>
       </c>
       <c r="F97" t="n">
-        <v>3.6793304517648335E-4</v>
+        <v>3.679330451764836E-4</v>
       </c>
     </row>
     <row r="98">
@@ -2717,7 +2717,7 @@
         <v>140900.0</v>
       </c>
       <c r="F98" t="n">
-        <v>3.505225356584713E-4</v>
+        <v>3.505225356584716E-4</v>
       </c>
     </row>
     <row r="99">
@@ -2737,7 +2737,7 @@
         <v>241400.0</v>
       </c>
       <c r="F99" t="n">
-        <v>3.411643748846318E-4</v>
+        <v>3.4116437488463205E-4</v>
       </c>
     </row>
     <row r="100">
@@ -2757,7 +2757,7 @@
         <v>148300.0</v>
       </c>
       <c r="F100" t="n">
-        <v>3.4108567508672744E-4</v>
+        <v>3.410856750867277E-4</v>
       </c>
     </row>
     <row r="101">
@@ -2777,7 +2777,7 @@
         <v>198000.0</v>
       </c>
       <c r="F101" t="n">
-        <v>3.2856659471996015E-4</v>
+        <v>3.285665947199604E-4</v>
       </c>
     </row>
     <row r="102">
@@ -2797,7 +2797,7 @@
         <v>543000.0</v>
       </c>
       <c r="F102" t="n">
-        <v>3.2823604260689336E-4</v>
+        <v>3.282360426068937E-4</v>
       </c>
     </row>
     <row r="103">
@@ -2817,7 +2817,7 @@
         <v>2900000.0</v>
       </c>
       <c r="F103" t="n">
-        <v>3.2649487653549765E-4</v>
+        <v>3.264948765354979E-4</v>
       </c>
     </row>
     <row r="104">
@@ -2837,7 +2837,7 @@
         <v>818600.0</v>
       </c>
       <c r="F104" t="n">
-        <v>3.1724561867124457E-4</v>
+        <v>3.1724561867124484E-4</v>
       </c>
     </row>
     <row r="105">
@@ -2857,7 +2857,7 @@
         <v>231900.0</v>
       </c>
       <c r="F105" t="n">
-        <v>2.927223951709339E-4</v>
+        <v>2.9272239517093415E-4</v>
       </c>
     </row>
     <row r="106">
@@ -2877,7 +2877,7 @@
         <v>310700.0</v>
       </c>
       <c r="F106" t="n">
-        <v>2.613301180496958E-4</v>
+        <v>2.613301180496961E-4</v>
       </c>
     </row>
     <row r="107">
@@ -2897,7 +2897,7 @@
         <v>1100000.0</v>
       </c>
       <c r="F107" t="n">
-        <v>2.332931630675543E-4</v>
+        <v>2.332931630675545E-4</v>
       </c>
     </row>
     <row r="108">
@@ -2917,7 +2917,7 @@
         <v>702500.0</v>
       </c>
       <c r="F108" t="n">
-        <v>2.3218077681752474E-4</v>
+        <v>2.3218077681752493E-4</v>
       </c>
     </row>
     <row r="109">
@@ -2937,7 +2937,7 @@
         <v>1000000.0</v>
       </c>
       <c r="F109" t="n">
-        <v>2.2752300685140197E-4</v>
+        <v>2.2752300685140221E-4</v>
       </c>
     </row>
     <row r="110">
@@ -2957,7 +2957,7 @@
         <v>1700000.0</v>
       </c>
       <c r="F110" t="n">
-        <v>2.2323837610376142E-4</v>
+        <v>2.2323837610376158E-4</v>
       </c>
     </row>
     <row r="111">
@@ -2977,7 +2977,7 @@
         <v>200300.0</v>
       </c>
       <c r="F111" t="n">
-        <v>2.1420205286809102E-4</v>
+        <v>2.142020528680912E-4</v>
       </c>
     </row>
     <row r="112">
@@ -2997,7 +2997,7 @@
         <v>270900.0</v>
       </c>
       <c r="F112" t="n">
-        <v>2.0419735638175476E-4</v>
+        <v>2.0419735638175493E-4</v>
       </c>
     </row>
     <row r="113">
@@ -3017,7 +3017,7 @@
         <v>186300.0</v>
       </c>
       <c r="F113" t="n">
-        <v>1.7874016123760222E-4</v>
+        <v>1.7874016123760238E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed Pagerank algorithm into a simpler version
</commit_message>
<xml_diff>
--- a/twitter-influencer-ranking/ranking_output.xlsx
+++ b/twitter-influencer-ranking/ranking_output.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="302">
   <si>
     <t>Rank</t>
   </si>
@@ -32,16 +32,52 @@
     <t>PageRank Score</t>
   </si>
   <si>
+    <t>Department of Government Efficiency</t>
+  </si>
+  <si>
+    <t>@DOGE</t>
+  </si>
+  <si>
     <t>Elon Musk</t>
   </si>
   <si>
     <t>@elonmusk</t>
   </si>
   <si>
-    <t>Department of Government Efficiency</t>
-  </si>
-  <si>
-    <t>@DOGE</t>
+    <t>Donald J. Trump</t>
+  </si>
+  <si>
+    <t>@realDonaldTrump</t>
+  </si>
+  <si>
+    <t>DEGEN NEWS</t>
+  </si>
+  <si>
+    <t>@DegenerateNews</t>
+  </si>
+  <si>
+    <t>Binance</t>
+  </si>
+  <si>
+    <t>@binance</t>
+  </si>
+  <si>
+    <t>Balaji</t>
+  </si>
+  <si>
+    <t>@balajis</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>@ton_blockchain</t>
+  </si>
+  <si>
+    <t>The Bearable Bull</t>
+  </si>
+  <si>
+    <t>@thebearablebull</t>
   </si>
   <si>
     <t>Solana</t>
@@ -50,28 +86,34 @@
     <t>@solana</t>
   </si>
   <si>
-    <t>DEGEN NEWS</t>
-  </si>
-  <si>
-    <t>@DegenerateNews</t>
-  </si>
-  <si>
-    <t>TON</t>
-  </si>
-  <si>
-    <t>@ton_blockchain</t>
-  </si>
-  <si>
-    <t>The Bearable Bull</t>
-  </si>
-  <si>
-    <t>@thebearablebull</t>
-  </si>
-  <si>
-    <t>Binance</t>
-  </si>
-  <si>
-    <t>@binance</t>
+    <t>Altcoin Daily</t>
+  </si>
+  <si>
+    <t>@AltcoinDailyio</t>
+  </si>
+  <si>
+    <t>David Sacks</t>
+  </si>
+  <si>
+    <t>@DavidSacks</t>
+  </si>
+  <si>
+    <t>Brad Garlinghouse</t>
+  </si>
+  <si>
+    <t>@bgarlinghouse</t>
+  </si>
+  <si>
+    <t>Crypto Rover</t>
+  </si>
+  <si>
+    <t>@rovercrc</t>
+  </si>
+  <si>
+    <t>WIZZ</t>
+  </si>
+  <si>
+    <t>@CryptoWizardd</t>
   </si>
   <si>
     <t>David "JoelKatz" Schwartz</t>
@@ -80,58 +122,190 @@
     <t>@JoelKatz</t>
   </si>
   <si>
-    <t>WIZZ</t>
-  </si>
-  <si>
-    <t>@CryptoWizardd</t>
-  </si>
-  <si>
-    <t>Altcoin Daily</t>
-  </si>
-  <si>
-    <t>@AltcoinDailyio</t>
-  </si>
-  <si>
-    <t>Brad Garlinghouse</t>
-  </si>
-  <si>
-    <t>@bgarlinghouse</t>
-  </si>
-  <si>
     <t>Crypto Tony</t>
   </si>
   <si>
     <t>@CryptoTony__</t>
   </si>
   <si>
+    <t>TechDev</t>
+  </si>
+  <si>
+    <t>@TechDev_52</t>
+  </si>
+  <si>
+    <t>The ₿itcoin Therapist</t>
+  </si>
+  <si>
+    <t>@TheBTCTherapist</t>
+  </si>
+  <si>
+    <t>Bitcoin Magazine</t>
+  </si>
+  <si>
+    <t>@BitcoinMagazine</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>@cz_binance</t>
+  </si>
+  <si>
+    <t>Brian Armstrong</t>
+  </si>
+  <si>
+    <t>@brian_armstrong</t>
+  </si>
+  <si>
+    <t>Galxe</t>
+  </si>
+  <si>
+    <t>@Galxe</t>
+  </si>
+  <si>
+    <t>ZachXBT</t>
+  </si>
+  <si>
+    <t>@zachxbt</t>
+  </si>
+  <si>
+    <t>The Moon Show</t>
+  </si>
+  <si>
+    <t>@TheMoonCarl</t>
+  </si>
+  <si>
+    <t>Sandeep (※,※)</t>
+  </si>
+  <si>
+    <t>@sandeepnailwal</t>
+  </si>
+  <si>
+    <t>Ice Open Network</t>
+  </si>
+  <si>
+    <t>@ice_blockchain</t>
+  </si>
+  <si>
+    <t>Michael Saylor</t>
+  </si>
+  <si>
+    <t>@saylor</t>
+  </si>
+  <si>
+    <t>XRPP</t>
+  </si>
+  <si>
+    <t>@XRP_Productions</t>
+  </si>
+  <si>
+    <t>Wormhole</t>
+  </si>
+  <si>
+    <t>@wormhole</t>
+  </si>
+  <si>
+    <t>MEXC</t>
+  </si>
+  <si>
+    <t>@MEXC_Official</t>
+  </si>
+  <si>
+    <t>Sergey Nazarov</t>
+  </si>
+  <si>
+    <t>@SergeyNazarov</t>
+  </si>
+  <si>
+    <t>Nayib Bukele</t>
+  </si>
+  <si>
+    <t>@nayibbukele</t>
+  </si>
+  <si>
+    <t>Marc Andreessen</t>
+  </si>
+  <si>
+    <t>@pmarca</t>
+  </si>
+  <si>
     <t>punya prasun bajpai</t>
   </si>
   <si>
     <t>@ppbajpai</t>
   </si>
   <si>
-    <t>ZachXBT</t>
-  </si>
-  <si>
-    <t>@zachxbt</t>
-  </si>
-  <si>
-    <t>Sergey Nazarov</t>
-  </si>
-  <si>
-    <t>@SergeyNazarov</t>
-  </si>
-  <si>
-    <t>Crypto Rover</t>
-  </si>
-  <si>
-    <t>@rovercrc</t>
-  </si>
-  <si>
-    <t>TechDev</t>
-  </si>
-  <si>
-    <t>@TechDev_52</t>
+    <t>CoinDesk</t>
+  </si>
+  <si>
+    <t>@CoinDesk</t>
+  </si>
+  <si>
+    <t>DeFi Princess | Storyteller</t>
+  </si>
+  <si>
+    <t>@defiprincess_</t>
+  </si>
+  <si>
+    <t>Cred</t>
+  </si>
+  <si>
+    <t>@CryptoCred</t>
+  </si>
+  <si>
+    <t>Alex Becker</t>
+  </si>
+  <si>
+    <t>@ZssBecker</t>
+  </si>
+  <si>
+    <t>Gate.io</t>
+  </si>
+  <si>
+    <t>@gate_io</t>
+  </si>
+  <si>
+    <t>PancakeSwap</t>
+  </si>
+  <si>
+    <t>@PancakeSwap</t>
+  </si>
+  <si>
+    <t>Crypto Tea</t>
+  </si>
+  <si>
+    <t>@CryptoTea_</t>
+  </si>
+  <si>
+    <t>Aethir</t>
+  </si>
+  <si>
+    <t>@AethirCloud</t>
+  </si>
+  <si>
+    <t>Optimism</t>
+  </si>
+  <si>
+    <t>@Optimism</t>
+  </si>
+  <si>
+    <t>Dogs Community</t>
+  </si>
+  <si>
+    <t>@realDogsHouse</t>
+  </si>
+  <si>
+    <t>TRON DAO</t>
+  </si>
+  <si>
+    <t>@trondao</t>
+  </si>
+  <si>
+    <t>Palmer Luckey</t>
+  </si>
+  <si>
+    <t>@PalmerLuckey</t>
   </si>
   <si>
     <t>Gordon</t>
@@ -140,124 +314,70 @@
     <t>@AltcoinGordon</t>
   </si>
   <si>
-    <t>XRPP</t>
-  </si>
-  <si>
-    <t>@XRP_Productions</t>
-  </si>
-  <si>
-    <t>The Moon Show</t>
-  </si>
-  <si>
-    <t>@TheMoonCarl</t>
-  </si>
-  <si>
-    <t>Bitcoin Magazine</t>
-  </si>
-  <si>
-    <t>@BitcoinMagazine</t>
-  </si>
-  <si>
-    <t>Brian Armstrong</t>
-  </si>
-  <si>
-    <t>@brian_armstrong</t>
-  </si>
-  <si>
-    <t>Galxe</t>
-  </si>
-  <si>
-    <t>@Galxe</t>
-  </si>
-  <si>
-    <t>Sandeep (※,※)</t>
-  </si>
-  <si>
-    <t>@sandeepnailwal</t>
-  </si>
-  <si>
-    <t>CZ</t>
-  </si>
-  <si>
-    <t>@cz_binance</t>
-  </si>
-  <si>
-    <t>TRON DAO</t>
-  </si>
-  <si>
-    <t>@trondao</t>
-  </si>
-  <si>
-    <t>Marc Andreessen</t>
-  </si>
-  <si>
-    <t>@pmarca</t>
-  </si>
-  <si>
-    <t>Balaji</t>
-  </si>
-  <si>
-    <t>@balajis</t>
-  </si>
-  <si>
-    <t>Cred</t>
-  </si>
-  <si>
-    <t>@CryptoCred</t>
-  </si>
-  <si>
-    <t>DeFi Princess | Storyteller</t>
-  </si>
-  <si>
-    <t>@defiprincess_</t>
-  </si>
-  <si>
     <t>Preston Pysh</t>
   </si>
   <si>
     <t>@PrestonPysh</t>
   </si>
   <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>@america</t>
+  </si>
+  <si>
+    <t>CRYPTO THRO</t>
+  </si>
+  <si>
+    <t>@CryptoThro</t>
+  </si>
+  <si>
+    <t>Ash Crypto</t>
+  </si>
+  <si>
+    <t>@Ashcryptoreal</t>
+  </si>
+  <si>
+    <t>Andrew Tate</t>
+  </si>
+  <si>
+    <t>@Cobratate</t>
+  </si>
+  <si>
+    <t>Bitget</t>
+  </si>
+  <si>
+    <t>@bitgetglobal</t>
+  </si>
+  <si>
+    <t>Wendy O</t>
+  </si>
+  <si>
+    <t>@CryptoWendyO</t>
+  </si>
+  <si>
+    <t>Bitcoin Archive</t>
+  </si>
+  <si>
+    <t>@BTC_Archive</t>
+  </si>
+  <si>
+    <t>Crypto.com</t>
+  </si>
+  <si>
+    <t>@cryptocom</t>
+  </si>
+  <si>
     <t>H.E. Justin Sun</t>
   </si>
   <si>
     <t>@justinsuntron</t>
   </si>
   <si>
-    <t>Dogs Community</t>
-  </si>
-  <si>
-    <t>@realDogsHouse</t>
-  </si>
-  <si>
-    <t>Optimism</t>
-  </si>
-  <si>
-    <t>@Optimism</t>
-  </si>
-  <si>
-    <t>Aethir</t>
-  </si>
-  <si>
-    <t>@AethirCloud</t>
-  </si>
-  <si>
-    <t>Alex Becker</t>
-  </si>
-  <si>
-    <t>@ZssBecker</t>
-  </si>
-  <si>
-    <t>Crypto Tea</t>
-  </si>
-  <si>
-    <t>@CryptoTea_</t>
-  </si>
-  <si>
-    <t>Andrew Tate</t>
-  </si>
-  <si>
-    <t>@Cobratate</t>
+    <t>CallFluentAI</t>
+  </si>
+  <si>
+    <t>@callfluentAI</t>
   </si>
   <si>
     <t>Mercek</t>
@@ -266,70 +386,244 @@
     <t>@WorldOfMercek</t>
   </si>
   <si>
+    <t>Coinbase</t>
+  </si>
+  <si>
+    <t>@coinbase</t>
+  </si>
+  <si>
+    <t>BNB Chain</t>
+  </si>
+  <si>
+    <t>@BNBCHAIN</t>
+  </si>
+  <si>
+    <t>MON Protocol</t>
+  </si>
+  <si>
+    <t>@monprotocol</t>
+  </si>
+  <si>
+    <t>Ivan on Tech</t>
+  </si>
+  <si>
+    <t>@IvanOnTech</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>@Vivek4real_</t>
+  </si>
+  <si>
+    <t>Adam Back</t>
+  </si>
+  <si>
+    <t>@adam3us</t>
+  </si>
+  <si>
+    <t>HEADBOY</t>
+  </si>
+  <si>
+    <t>@NDIDI_GRAM</t>
+  </si>
+  <si>
+    <t>Supra</t>
+  </si>
+  <si>
+    <t>@SUPRA_Labs</t>
+  </si>
+  <si>
+    <t>sanyi.eth</t>
+  </si>
+  <si>
+    <t>@sanyi_eth_</t>
+  </si>
+  <si>
+    <t>Confidential Layer</t>
+  </si>
+  <si>
+    <t>@ConfidentialLyr</t>
+  </si>
+  <si>
+    <t>RoOLZ</t>
+  </si>
+  <si>
+    <t>@Roolznft</t>
+  </si>
+  <si>
+    <t>Soneium</t>
+  </si>
+  <si>
+    <t>@soneium</t>
+  </si>
+  <si>
+    <t>whale</t>
+  </si>
+  <si>
+    <t>@cardano_whale</t>
+  </si>
+  <si>
+    <t>Nature is Amazing</t>
+  </si>
+  <si>
+    <t>@AMAZlNGNATURE</t>
+  </si>
+  <si>
     <t>Abstract</t>
   </si>
   <si>
     <t>@AbstractChain</t>
   </si>
   <si>
-    <t>Gate.io</t>
-  </si>
-  <si>
-    <t>@gate_io</t>
-  </si>
-  <si>
-    <t>MEXC</t>
-  </si>
-  <si>
-    <t>@MEXC_Official</t>
-  </si>
-  <si>
-    <t>CRYPTO THRO</t>
-  </si>
-  <si>
-    <t>@CryptoThro</t>
-  </si>
-  <si>
-    <t>Soneium</t>
-  </si>
-  <si>
-    <t>@soneium</t>
-  </si>
-  <si>
-    <t>America</t>
-  </si>
-  <si>
-    <t>@america</t>
-  </si>
-  <si>
-    <t>Ice Open Network</t>
-  </si>
-  <si>
-    <t>@ice_blockchain</t>
-  </si>
-  <si>
-    <t>Bitget</t>
-  </si>
-  <si>
-    <t>@bitgetglobal</t>
-  </si>
-  <si>
-    <t>Wormhole</t>
-  </si>
-  <si>
-    <t>@wormhole</t>
-  </si>
-  <si>
-    <t>PancakeSwap</t>
-  </si>
-  <si>
-    <t>@PancakeSwap</t>
-  </si>
-  <si>
-    <t>David Sacks</t>
-  </si>
-  <si>
-    <t>@DavidSacks</t>
+    <t>Avalanche9000</t>
+  </si>
+  <si>
+    <t>@avax</t>
+  </si>
+  <si>
+    <t>Stellar</t>
+  </si>
+  <si>
+    <t>@StellarOrg</t>
+  </si>
+  <si>
+    <t>CyrilXBT</t>
+  </si>
+  <si>
+    <t>@cyrilXBT</t>
+  </si>
+  <si>
+    <t>Memes Lab</t>
+  </si>
+  <si>
+    <t>@memeslabxyz</t>
+  </si>
+  <si>
+    <t>PAWS CULT</t>
+  </si>
+  <si>
+    <t>@PawsUpCult</t>
+  </si>
+  <si>
+    <t>Astra Nova</t>
+  </si>
+  <si>
+    <t>@Astra__Nova</t>
+  </si>
+  <si>
+    <t>DoctorX</t>
+  </si>
+  <si>
+    <t>@DoctorX_Meme</t>
+  </si>
+  <si>
+    <t>CARV</t>
+  </si>
+  <si>
+    <t>@carv_official</t>
+  </si>
+  <si>
+    <t>Cluster Protocol</t>
+  </si>
+  <si>
+    <t>@ClusterProtocol</t>
+  </si>
+  <si>
+    <t>Historic Vids</t>
+  </si>
+  <si>
+    <t>@historyinmemes</t>
+  </si>
+  <si>
+    <t>KiloEx</t>
+  </si>
+  <si>
+    <t>@KiloEx_perp</t>
+  </si>
+  <si>
+    <t>Jacob King</t>
+  </si>
+  <si>
+    <t>@JacobKinge</t>
+  </si>
+  <si>
+    <t>Erik Voorhees</t>
+  </si>
+  <si>
+    <t>@ErikVoorhees</t>
+  </si>
+  <si>
+    <t>Jason A. Williams</t>
+  </si>
+  <si>
+    <t>@GoingParabolic</t>
+  </si>
+  <si>
+    <t>van00sa</t>
+  </si>
+  <si>
+    <t>@van00sa</t>
+  </si>
+  <si>
+    <t>Lex Fridman</t>
+  </si>
+  <si>
+    <t>@lexfridman</t>
+  </si>
+  <si>
+    <t>Lingo</t>
+  </si>
+  <si>
+    <t>@Lingocoins</t>
+  </si>
+  <si>
+    <t>0xNobler</t>
+  </si>
+  <si>
+    <t>@CryptoNobler</t>
+  </si>
+  <si>
+    <t>DeBank</t>
+  </si>
+  <si>
+    <t>@DeBankDeFi</t>
+  </si>
+  <si>
+    <t>Interesting As Fuck</t>
+  </si>
+  <si>
+    <t>@interesting_aIl</t>
+  </si>
+  <si>
+    <t>Phantom</t>
+  </si>
+  <si>
+    <t>@phantom</t>
+  </si>
+  <si>
+    <t>Radar</t>
+  </si>
+  <si>
+    <t>@RadarHits</t>
+  </si>
+  <si>
+    <t>Uphold</t>
+  </si>
+  <si>
+    <t>@UpholdInc</t>
+  </si>
+  <si>
+    <t>FearBuck</t>
+  </si>
+  <si>
+    <t>@FearedBuck</t>
+  </si>
+  <si>
+    <t>BITCOINLFG®</t>
+  </si>
+  <si>
+    <t>@bitcoinlfgo</t>
   </si>
   <si>
     <t>Coach Bruce (kween/acc)</t>
@@ -338,130 +632,28 @@
     <t>@OX_DAO</t>
   </si>
   <si>
-    <t>DeBank</t>
-  </si>
-  <si>
-    <t>@DeBankDeFi</t>
-  </si>
-  <si>
-    <t>KiloEx</t>
-  </si>
-  <si>
-    <t>@KiloEx_perp</t>
-  </si>
-  <si>
-    <t>Ivan on Tech</t>
-  </si>
-  <si>
-    <t>@IvanOnTech</t>
-  </si>
-  <si>
-    <t>HEADBOY</t>
-  </si>
-  <si>
-    <t>@NDIDI_GRAM</t>
-  </si>
-  <si>
-    <t>whale</t>
-  </si>
-  <si>
-    <t>@cardano_whale</t>
-  </si>
-  <si>
-    <t>Wendy O</t>
-  </si>
-  <si>
-    <t>@CryptoWendyO</t>
-  </si>
-  <si>
-    <t>Coinbase</t>
-  </si>
-  <si>
-    <t>@coinbase</t>
-  </si>
-  <si>
-    <t>BNB Chain</t>
-  </si>
-  <si>
-    <t>@BNBCHAIN</t>
-  </si>
-  <si>
-    <t>Ash Crypto</t>
-  </si>
-  <si>
-    <t>@Ashcryptoreal</t>
-  </si>
-  <si>
-    <t>Cluster Protocol</t>
-  </si>
-  <si>
-    <t>@ClusterProtocol</t>
-  </si>
-  <si>
-    <t>Supra</t>
-  </si>
-  <si>
-    <t>@SUPRA_Labs</t>
-  </si>
-  <si>
-    <t>The ₿itcoin Therapist</t>
-  </si>
-  <si>
-    <t>@TheBTCTherapist</t>
-  </si>
-  <si>
-    <t>Nayib Bukele</t>
-  </si>
-  <si>
-    <t>@nayibbukele</t>
-  </si>
-  <si>
-    <t>Jason A. Williams</t>
-  </si>
-  <si>
-    <t>@GoingParabolic</t>
-  </si>
-  <si>
-    <t>Confidential Layer</t>
-  </si>
-  <si>
-    <t>@ConfidentialLyr</t>
-  </si>
-  <si>
-    <t>Stellar</t>
-  </si>
-  <si>
-    <t>@StellarOrg</t>
-  </si>
-  <si>
-    <t>Nature is Amazing</t>
-  </si>
-  <si>
-    <t>@AMAZlNGNATURE</t>
-  </si>
-  <si>
-    <t>Crypto.com</t>
-  </si>
-  <si>
-    <t>@cryptocom</t>
-  </si>
-  <si>
-    <t>CyrilXBT</t>
-  </si>
-  <si>
-    <t>@cyrilXBT</t>
-  </si>
-  <si>
-    <t>BITCOINLFG®</t>
-  </si>
-  <si>
-    <t>@bitcoinlfgo</t>
-  </si>
-  <si>
-    <t>Avalanche9000</t>
-  </si>
-  <si>
-    <t>@avax</t>
+    <t>DuckChain</t>
+  </si>
+  <si>
+    <t>@Duck_Chain</t>
+  </si>
+  <si>
+    <t>Baby Doge</t>
+  </si>
+  <si>
+    <t>@BabyDogeCoin</t>
+  </si>
+  <si>
+    <t>xMoney.com</t>
+  </si>
+  <si>
+    <t>@xMoney_com</t>
+  </si>
+  <si>
+    <t>Lyn Alden</t>
+  </si>
+  <si>
+    <t>@LynAldenContact</t>
   </si>
   <si>
     <t>Artyfact</t>
@@ -470,22 +662,100 @@
     <t>@artyfact_game</t>
   </si>
   <si>
-    <t>van00sa</t>
-  </si>
-  <si>
-    <t>@van00sa</t>
-  </si>
-  <si>
-    <t>Historic Vids</t>
-  </si>
-  <si>
-    <t>@historyinmemes</t>
-  </si>
-  <si>
-    <t>Jacob King</t>
-  </si>
-  <si>
-    <t>@JacobKinge</t>
+    <t>Bitget Wallet</t>
+  </si>
+  <si>
+    <t>@BitgetWallet</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>@fuelkek</t>
+  </si>
+  <si>
+    <t>Ian Jaeger</t>
+  </si>
+  <si>
+    <t>@IanJaeger29</t>
+  </si>
+  <si>
+    <t>MANTRA | Mainnet Live</t>
+  </si>
+  <si>
+    <t>@MANTRA_Chain</t>
+  </si>
+  <si>
+    <t>Yescoin</t>
+  </si>
+  <si>
+    <t>@Yescoin_Fam</t>
+  </si>
+  <si>
+    <t>Everything Georgia</t>
+  </si>
+  <si>
+    <t>@GAFollowers</t>
+  </si>
+  <si>
+    <t>Mnemonics_coin</t>
+  </si>
+  <si>
+    <t>@Mnemonics_coin</t>
+  </si>
+  <si>
+    <t>American AF</t>
+  </si>
+  <si>
+    <t>@iAnonPatriot</t>
+  </si>
+  <si>
+    <t>Tom Woods</t>
+  </si>
+  <si>
+    <t>@ThomasEWoods</t>
+  </si>
+  <si>
+    <t>Chris Pavlovski</t>
+  </si>
+  <si>
+    <t>@chrispavlovski</t>
+  </si>
+  <si>
+    <t>dubzy</t>
+  </si>
+  <si>
+    <t>@dubzyxbt</t>
+  </si>
+  <si>
+    <t>Donald J. Trump News</t>
+  </si>
+  <si>
+    <t>@realTrumpNewsX</t>
+  </si>
+  <si>
+    <t>Jack Poso</t>
+  </si>
+  <si>
+    <t>@JackPosobiec</t>
+  </si>
+  <si>
+    <t>Wimar.X</t>
+  </si>
+  <si>
+    <t>@DefiWimar</t>
+  </si>
+  <si>
+    <t>Sulaiman Ahmed</t>
+  </si>
+  <si>
+    <t>@ShaykhSulaiman</t>
+  </si>
+  <si>
+    <t>Peter Schiff</t>
+  </si>
+  <si>
+    <t>@PeterSchiff</t>
   </si>
   <si>
     <t>gaut</t>
@@ -494,28 +764,22 @@
     <t>@0xgaut</t>
   </si>
   <si>
-    <t>Baby Doge</t>
-  </si>
-  <si>
-    <t>@BabyDogeCoin</t>
-  </si>
-  <si>
-    <t>Uphold</t>
-  </si>
-  <si>
-    <t>@UpholdInc</t>
-  </si>
-  <si>
-    <t>Lingo</t>
-  </si>
-  <si>
-    <t>@Lingocoins</t>
-  </si>
-  <si>
-    <t>Donald J. Trump News</t>
-  </si>
-  <si>
-    <t>@realTrumpNewsX</t>
+    <t>Not Jerome Powell</t>
+  </si>
+  <si>
+    <t>@alifarhat79</t>
+  </si>
+  <si>
+    <t>हर्ष वर्धन त्रिपाठी</t>
+  </si>
+  <si>
+    <t>@MediaHarshVT</t>
+  </si>
+  <si>
+    <t>Mandy</t>
+  </si>
+  <si>
+    <t>@MarindaVannoy1</t>
   </si>
   <si>
     <t>BFDCoin</t>
@@ -524,64 +788,64 @@
     <t>@BFDCoin</t>
   </si>
   <si>
-    <t>xMoney.com</t>
-  </si>
-  <si>
-    <t>@xMoney_com</t>
-  </si>
-  <si>
-    <t>Lex Fridman</t>
-  </si>
-  <si>
-    <t>@lexfridman</t>
-  </si>
-  <si>
-    <t>Mnemonics_coin</t>
-  </si>
-  <si>
-    <t>@Mnemonics_coin</t>
-  </si>
-  <si>
-    <t>DuckChain</t>
-  </si>
-  <si>
-    <t>@Duck_Chain</t>
-  </si>
-  <si>
-    <t>Phantom</t>
-  </si>
-  <si>
-    <t>@phantom</t>
-  </si>
-  <si>
-    <t>0xNobler</t>
-  </si>
-  <si>
-    <t>@CryptoNobler</t>
-  </si>
-  <si>
-    <t>MANTRA | Mainnet Live</t>
-  </si>
-  <si>
-    <t>@MANTRA_Chain</t>
-  </si>
-  <si>
-    <t>dubzy</t>
-  </si>
-  <si>
-    <t>@dubzyxbt</t>
-  </si>
-  <si>
-    <t>Radar</t>
-  </si>
-  <si>
-    <t>@RadarHits</t>
-  </si>
-  <si>
-    <t>Bitget Wallet</t>
-  </si>
-  <si>
-    <t>@BitgetWallet</t>
+    <t>Jonathan Chang</t>
+  </si>
+  <si>
+    <t>@0xjyjonathan</t>
+  </si>
+  <si>
+    <t>Somos Cosmos</t>
+  </si>
+  <si>
+    <t>@InformaCosmos</t>
+  </si>
+  <si>
+    <t>Leonidas $DOG</t>
+  </si>
+  <si>
+    <t>@LeonidasNFT</t>
+  </si>
+  <si>
+    <t>Revolving Games</t>
+  </si>
+  <si>
+    <t>@Revolving_Games</t>
+  </si>
+  <si>
+    <t>Tyrese Maxey</t>
+  </si>
+  <si>
+    <t>@TyreseMaxey</t>
+  </si>
+  <si>
+    <t>Ravish Kumar ᴾᵃʳᵒᵈʸ ©</t>
+  </si>
+  <si>
+    <t>@SirRavishFC</t>
+  </si>
+  <si>
+    <t>Cristiano Ronaldo</t>
+  </si>
+  <si>
+    <t>@Cristiano</t>
+  </si>
+  <si>
+    <t>ORA</t>
+  </si>
+  <si>
+    <t>@OraProtocol</t>
+  </si>
+  <si>
+    <t>عبدالعزيز أحمد بغلف</t>
+  </si>
+  <si>
+    <t>@AzizbagBag</t>
+  </si>
+  <si>
+    <t>HOW THINGS WORK</t>
+  </si>
+  <si>
+    <t>@HowThingsWork_</t>
   </si>
   <si>
     <t>Slingshot DAO</t>
@@ -590,36 +854,6 @@
     <t>@SlingshotDAO</t>
   </si>
   <si>
-    <t>Wimar.X</t>
-  </si>
-  <si>
-    <t>@DefiWimar</t>
-  </si>
-  <si>
-    <t>Revolving Games</t>
-  </si>
-  <si>
-    <t>@Revolving_Games</t>
-  </si>
-  <si>
-    <t>Ravish Kumar ᴾᵃʳᵒᵈʸ ©</t>
-  </si>
-  <si>
-    <t>@SirRavishFC</t>
-  </si>
-  <si>
-    <t>हर्ष वर्धन त्रिपाठी</t>
-  </si>
-  <si>
-    <t>@MediaHarshVT</t>
-  </si>
-  <si>
-    <t>Leonidas $DOG</t>
-  </si>
-  <si>
-    <t>@LeonidasNFT</t>
-  </si>
-  <si>
     <t>Unite</t>
   </si>
   <si>
@@ -632,28 +866,16 @@
     <t>@saakuru_labs</t>
   </si>
   <si>
-    <t>Not Jerome Powell</t>
-  </si>
-  <si>
-    <t>@alifarhat79</t>
-  </si>
-  <si>
-    <t>Jack Poso</t>
-  </si>
-  <si>
-    <t>@JackPosobiec</t>
-  </si>
-  <si>
-    <t>عبدالعزيز أحمد بغلف</t>
-  </si>
-  <si>
-    <t>@AzizbagBag</t>
-  </si>
-  <si>
-    <t>Astra Nova</t>
-  </si>
-  <si>
-    <t>@Astra__Nova</t>
+    <t>Arena Games</t>
+  </si>
+  <si>
+    <t>@Arenaweb3</t>
+  </si>
+  <si>
+    <t>CITY Holder</t>
+  </si>
+  <si>
+    <t>@city_holder</t>
   </si>
   <si>
     <t>Tari</t>
@@ -662,34 +884,40 @@
     <t>@tari</t>
   </si>
   <si>
+    <t>Rami Ismail / رامي</t>
+  </si>
+  <si>
+    <t>@tha_rami</t>
+  </si>
+  <si>
+    <t>Crypto Valley Exchange (CVEX)</t>
+  </si>
+  <si>
+    <t>@cvex_xyz</t>
+  </si>
+  <si>
+    <t>AstrArk</t>
+  </si>
+  <si>
+    <t>@AstrArk_World</t>
+  </si>
+  <si>
     <t>POWR</t>
   </si>
   <si>
     <t>@POWReSports</t>
   </si>
   <si>
-    <t>Peter Schiff</t>
-  </si>
-  <si>
-    <t>@PeterSchiff</t>
-  </si>
-  <si>
-    <t>Everything Georgia</t>
-  </si>
-  <si>
-    <t>@GAFollowers</t>
-  </si>
-  <si>
-    <t>Rami Ismail / رامي</t>
-  </si>
-  <si>
-    <t>@tha_rami</t>
-  </si>
-  <si>
-    <t>Arena Games</t>
-  </si>
-  <si>
-    <t>@Arenaweb3</t>
+    <t>BRS Party</t>
+  </si>
+  <si>
+    <t>@BRSparty</t>
+  </si>
+  <si>
+    <t>Marcel</t>
+  </si>
+  <si>
+    <t>@realmarcel1</t>
   </si>
 </sst>
 </file>
@@ -734,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -773,7 +1001,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>1062.0</v>
+        <v>1064.0</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -782,10 +1010,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>2.067E8</v>
+        <v>2300000.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.005212370858161699</v>
+        <v>0.006691337778661934</v>
       </c>
     </row>
     <row r="3">
@@ -793,7 +1021,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1064.0</v>
+        <v>1062.0</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -802,10 +1030,10 @@
         <v>9</v>
       </c>
       <c r="E3" t="n">
-        <v>2300000.0</v>
+        <v>2.067E8</v>
       </c>
       <c r="F3" t="n">
-        <v>0.005114974833389286</v>
+        <v>0.005250926464844939</v>
       </c>
     </row>
     <row r="4">
@@ -813,7 +1041,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="n">
-        <v>1085.0</v>
+        <v>1480.0</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -822,10 +1050,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>2900000.0</v>
+        <v>9.58E7</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0047579488518522</v>
+        <v>0.005170866141226624</v>
       </c>
     </row>
     <row r="5">
@@ -845,7 +1073,7 @@
         <v>292300.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.004657683433566352</v>
+        <v>0.004281758995644569</v>
       </c>
     </row>
     <row r="6">
@@ -853,7 +1081,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="n">
-        <v>11.0</v>
+        <v>706.0</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -862,10 +1090,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>2500000.0</v>
+        <v>1.37E7</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0038482392882576945</v>
+        <v>0.0042346729586932984</v>
       </c>
     </row>
     <row r="7">
@@ -873,7 +1101,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="n">
-        <v>1078.0</v>
+        <v>126.0</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -882,10 +1110,10 @@
         <v>17</v>
       </c>
       <c r="E7" t="n">
-        <v>326800.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0037639615166252353</v>
+        <v>0.0037552300066773306</v>
       </c>
     </row>
     <row r="8">
@@ -893,7 +1121,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="n">
-        <v>706.0</v>
+        <v>11.0</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -902,10 +1130,10 @@
         <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>1.37E7</v>
+        <v>2500000.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0035836810986542597</v>
+        <v>0.0036763417412184226</v>
       </c>
     </row>
     <row r="9">
@@ -913,7 +1141,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="n">
-        <v>1080.0</v>
+        <v>1078.0</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -922,10 +1150,10 @@
         <v>21</v>
       </c>
       <c r="E9" t="n">
-        <v>536900.0</v>
+        <v>326800.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.003526613244580157</v>
+        <v>0.0036706382439979754</v>
       </c>
     </row>
     <row r="10">
@@ -933,7 +1161,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="n">
-        <v>1069.0</v>
+        <v>1085.0</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -942,10 +1170,10 @@
         <v>23</v>
       </c>
       <c r="E10" t="n">
-        <v>755500.0</v>
+        <v>2900000.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0034530992777783943</v>
+        <v>0.003612254948504055</v>
       </c>
     </row>
     <row r="11">
@@ -965,7 +1193,7 @@
         <v>1700000.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0034507826875832585</v>
+        <v>0.0035927376845694818</v>
       </c>
     </row>
     <row r="12">
@@ -973,7 +1201,7 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="n">
-        <v>1111.0</v>
+        <v>1267.0</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
@@ -982,10 +1210,10 @@
         <v>27</v>
       </c>
       <c r="E12" t="n">
-        <v>940500.0</v>
+        <v>1100000.0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0034437753623922955</v>
+        <v>0.0035651111074312554</v>
       </c>
     </row>
     <row r="13">
@@ -993,7 +1221,7 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="n">
-        <v>1081.0</v>
+        <v>1111.0</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -1002,10 +1230,10 @@
         <v>29</v>
       </c>
       <c r="E13" t="n">
-        <v>479000.0</v>
+        <v>940500.0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0032915422651181763</v>
+        <v>0.0034009738173969195</v>
       </c>
     </row>
     <row r="14">
@@ -1013,7 +1241,7 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="n">
-        <v>805.0</v>
+        <v>8.0</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -1022,10 +1250,10 @@
         <v>31</v>
       </c>
       <c r="E14" t="n">
-        <v>2600000.0</v>
+        <v>980000.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0031854226147749838</v>
+        <v>0.0033433925458501977</v>
       </c>
     </row>
     <row r="15">
@@ -1033,7 +1261,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="n">
-        <v>1136.0</v>
+        <v>1069.0</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -1042,10 +1270,10 @@
         <v>33</v>
       </c>
       <c r="E15" t="n">
-        <v>705900.0</v>
+        <v>755500.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0030844683337041497</v>
+        <v>0.0033340218807577223</v>
       </c>
     </row>
     <row r="16">
@@ -1053,7 +1281,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="n">
-        <v>301.0</v>
+        <v>1080.0</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -1062,10 +1290,10 @@
         <v>35</v>
       </c>
       <c r="E16" t="n">
-        <v>152400.0</v>
+        <v>536900.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0028680092535308906</v>
+        <v>0.003258216521660335</v>
       </c>
     </row>
     <row r="17">
@@ -1073,7 +1301,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="n">
-        <v>8.0</v>
+        <v>1081.0</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -1082,10 +1310,10 @@
         <v>37</v>
       </c>
       <c r="E17" t="n">
-        <v>980000.0</v>
+        <v>479000.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.002814897073133077</v>
+        <v>0.0030588447325649534</v>
       </c>
     </row>
     <row r="18">
@@ -1105,7 +1333,7 @@
         <v>487700.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.002792019684221689</v>
+        <v>0.0030414529892869428</v>
       </c>
     </row>
     <row r="19">
@@ -1113,7 +1341,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="n">
-        <v>42.0</v>
+        <v>104.0</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -1122,10 +1350,10 @@
         <v>41</v>
       </c>
       <c r="E19" t="n">
-        <v>489700.0</v>
+        <v>166400.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0027762144738654486</v>
+        <v>0.0029047373594524827</v>
       </c>
     </row>
     <row r="20">
@@ -1133,7 +1361,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="n">
-        <v>1077.0</v>
+        <v>10.0</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
@@ -1142,10 +1370,10 @@
         <v>43</v>
       </c>
       <c r="E20" t="n">
-        <v>173200.0</v>
+        <v>3400000.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.002747967914016854</v>
+        <v>0.002836653054074937</v>
       </c>
     </row>
     <row r="21">
@@ -1153,7 +1381,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="n">
-        <v>1083.0</v>
+        <v>1063.0</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
@@ -1162,10 +1390,10 @@
         <v>45</v>
       </c>
       <c r="E21" t="n">
-        <v>1400000.0</v>
+        <v>9100000.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.002613561906329402</v>
+        <v>0.0028082263009243046</v>
       </c>
     </row>
     <row r="22">
@@ -1173,7 +1401,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="n">
-        <v>10.0</v>
+        <v>1125.0</v>
       </c>
       <c r="C22" t="s">
         <v>46</v>
@@ -1182,10 +1410,10 @@
         <v>47</v>
       </c>
       <c r="E22" t="n">
-        <v>3400000.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0026059317647641874</v>
+        <v>0.002738444420996268</v>
       </c>
     </row>
     <row r="23">
@@ -1193,7 +1421,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="n">
-        <v>1125.0</v>
+        <v>1108.0</v>
       </c>
       <c r="C23" t="s">
         <v>48</v>
@@ -1202,10 +1430,10 @@
         <v>49</v>
       </c>
       <c r="E23" t="n">
-        <v>1400000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0026038238521282845</v>
+        <v>0.002727137818098633</v>
       </c>
     </row>
     <row r="24">
@@ -1213,7 +1441,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="n">
-        <v>1108.0</v>
+        <v>1136.0</v>
       </c>
       <c r="C24" t="s">
         <v>50</v>
@@ -1222,10 +1450,10 @@
         <v>51</v>
       </c>
       <c r="E24" t="n">
-        <v>1500000.0</v>
+        <v>705900.0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.002568710031672654</v>
+        <v>0.002526137134740461</v>
       </c>
     </row>
     <row r="25">
@@ -1233,7 +1461,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="n">
-        <v>1166.0</v>
+        <v>1083.0</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
@@ -1242,10 +1470,10 @@
         <v>53</v>
       </c>
       <c r="E25" t="n">
-        <v>331500.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0025375882208780952</v>
+        <v>0.0025213194481636214</v>
       </c>
     </row>
     <row r="26">
@@ -1253,7 +1481,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="n">
-        <v>1063.0</v>
+        <v>1166.0</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
@@ -1262,10 +1490,10 @@
         <v>55</v>
       </c>
       <c r="E26" t="n">
-        <v>9100000.0</v>
+        <v>331500.0</v>
       </c>
       <c r="F26" t="n">
-        <v>0.002514245582511407</v>
+        <v>0.0024936609013582137</v>
       </c>
     </row>
     <row r="27">
@@ -1273,7 +1501,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="n">
-        <v>1091.0</v>
+        <v>13.0</v>
       </c>
       <c r="C27" t="s">
         <v>56</v>
@@ -1282,10 +1510,10 @@
         <v>57</v>
       </c>
       <c r="E27" t="n">
-        <v>1600000.0</v>
+        <v>2800000.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.002385674637786332</v>
+        <v>0.0024737367702927764</v>
       </c>
     </row>
     <row r="28">
@@ -1293,7 +1521,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="n">
-        <v>1223.0</v>
+        <v>1423.0</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
@@ -1302,10 +1530,10 @@
         <v>59</v>
       </c>
       <c r="E28" t="n">
-        <v>1600000.0</v>
+        <v>3800000.0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.002371424596276455</v>
+        <v>0.002463382647362269</v>
       </c>
     </row>
     <row r="29">
@@ -1313,7 +1541,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="n">
-        <v>126.0</v>
+        <v>1077.0</v>
       </c>
       <c r="C29" t="s">
         <v>60</v>
@@ -1322,10 +1550,10 @@
         <v>61</v>
       </c>
       <c r="E29" t="n">
-        <v>1000000.0</v>
+        <v>173200.0</v>
       </c>
       <c r="F29" t="n">
-        <v>0.002279939198611741</v>
+        <v>0.002451586721162212</v>
       </c>
     </row>
     <row r="30">
@@ -1333,7 +1561,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="n">
-        <v>1150.0</v>
+        <v>237.0</v>
       </c>
       <c r="C30" t="s">
         <v>62</v>
@@ -1342,10 +1570,10 @@
         <v>63</v>
       </c>
       <c r="E30" t="n">
-        <v>666500.0</v>
+        <v>373100.0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0022315561503877595</v>
+        <v>0.002429860326212977</v>
       </c>
     </row>
     <row r="31">
@@ -1353,7 +1581,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="n">
-        <v>1219.0</v>
+        <v>1070.0</v>
       </c>
       <c r="C31" t="s">
         <v>64</v>
@@ -1362,10 +1590,10 @@
         <v>65</v>
       </c>
       <c r="E31" t="n">
-        <v>137100.0</v>
+        <v>1400000.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0022315415753809817</v>
+        <v>0.0024081004674614604</v>
       </c>
     </row>
     <row r="32">
@@ -1373,7 +1601,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="n">
-        <v>1250.0</v>
+        <v>301.0</v>
       </c>
       <c r="C32" t="s">
         <v>66</v>
@@ -1382,10 +1610,10 @@
         <v>67</v>
       </c>
       <c r="E32" t="n">
-        <v>526600.0</v>
+        <v>152400.0</v>
       </c>
       <c r="F32" t="n">
-        <v>0.0021852708754264683</v>
+        <v>0.002378940417444737</v>
       </c>
     </row>
     <row r="33">
@@ -1393,7 +1621,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="n">
-        <v>1146.0</v>
+        <v>1222.0</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
@@ -1402,10 +1630,10 @@
         <v>69</v>
       </c>
       <c r="E33" t="n">
-        <v>3700000.0</v>
+        <v>6700000.0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.0021558502573102876</v>
+        <v>0.0023538185444479274</v>
       </c>
     </row>
     <row r="34">
@@ -1413,7 +1641,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="n">
-        <v>1224.0</v>
+        <v>1223.0</v>
       </c>
       <c r="C34" t="s">
         <v>70</v>
@@ -1422,10 +1650,10 @@
         <v>71</v>
       </c>
       <c r="E34" t="n">
-        <v>3500000.0</v>
+        <v>1600000.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0021434947680976078</v>
+        <v>0.002310255815739172</v>
       </c>
     </row>
     <row r="35">
@@ -1433,7 +1661,7 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="n">
-        <v>1142.0</v>
+        <v>805.0</v>
       </c>
       <c r="C35" t="s">
         <v>72</v>
@@ -1442,10 +1670,10 @@
         <v>73</v>
       </c>
       <c r="E35" t="n">
-        <v>715800.0</v>
+        <v>2600000.0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0021138311068041827</v>
+        <v>0.002188847874852732</v>
       </c>
     </row>
     <row r="36">
@@ -1453,7 +1681,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="n">
-        <v>1149.0</v>
+        <v>1698.0</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
@@ -1462,10 +1690,10 @@
         <v>75</v>
       </c>
       <c r="E36" t="n">
-        <v>852900.0</v>
+        <v>3200000.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.002039188203855036</v>
+        <v>0.0021856780561759722</v>
       </c>
     </row>
     <row r="37">
@@ -1473,7 +1701,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="n">
-        <v>1182.0</v>
+        <v>1219.0</v>
       </c>
       <c r="C37" t="s">
         <v>76</v>
@@ -1482,10 +1710,10 @@
         <v>77</v>
       </c>
       <c r="E37" t="n">
-        <v>1100000.0</v>
+        <v>137100.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.002035829018777899</v>
+        <v>0.0021611630923208417</v>
       </c>
     </row>
     <row r="38">
@@ -1493,7 +1721,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="n">
-        <v>3.0</v>
+        <v>1150.0</v>
       </c>
       <c r="C38" t="s">
         <v>78</v>
@@ -1502,10 +1730,10 @@
         <v>79</v>
       </c>
       <c r="E38" t="n">
-        <v>155900.0</v>
+        <v>666500.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.002011329523450835</v>
+        <v>0.0021537591167428097</v>
       </c>
     </row>
     <row r="39">
@@ -1513,7 +1741,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="n">
-        <v>1097.0</v>
+        <v>1182.0</v>
       </c>
       <c r="C39" t="s">
         <v>80</v>
@@ -1522,10 +1750,10 @@
         <v>81</v>
       </c>
       <c r="E39" t="n">
-        <v>1.04E7</v>
+        <v>1100000.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0019972560443486387</v>
+        <v>0.0021384590525133757</v>
       </c>
     </row>
     <row r="40">
@@ -1533,7 +1761,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="n">
-        <v>1211.0</v>
+        <v>1084.0</v>
       </c>
       <c r="C40" t="s">
         <v>82</v>
@@ -1542,10 +1770,10 @@
         <v>83</v>
       </c>
       <c r="E40" t="n">
-        <v>100400.0</v>
+        <v>2100000.0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0018956891057825458</v>
+        <v>0.0021160450282494622</v>
       </c>
     </row>
     <row r="41">
@@ -1553,7 +1781,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="n">
-        <v>20.0</v>
+        <v>1200.0</v>
       </c>
       <c r="C41" t="s">
         <v>84</v>
@@ -1562,10 +1790,10 @@
         <v>85</v>
       </c>
       <c r="E41" t="n">
-        <v>260500.0</v>
+        <v>2000000.0</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0018870705334992184</v>
+        <v>0.0021096797710982787</v>
       </c>
     </row>
     <row r="42">
@@ -1573,7 +1801,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="n">
-        <v>1084.0</v>
+        <v>3.0</v>
       </c>
       <c r="C42" t="s">
         <v>86</v>
@@ -1582,10 +1810,10 @@
         <v>87</v>
       </c>
       <c r="E42" t="n">
-        <v>2100000.0</v>
+        <v>155900.0</v>
       </c>
       <c r="F42" t="n">
-        <v>0.001881593981158707</v>
+        <v>0.002031367209535331</v>
       </c>
     </row>
     <row r="43">
@@ -1593,7 +1821,7 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="n">
-        <v>1070.0</v>
+        <v>1149.0</v>
       </c>
       <c r="C43" t="s">
         <v>88</v>
@@ -1602,10 +1830,10 @@
         <v>89</v>
       </c>
       <c r="E43" t="n">
-        <v>1400000.0</v>
+        <v>852900.0</v>
       </c>
       <c r="F43" t="n">
-        <v>0.0018059738277655083</v>
+        <v>0.0020158131853527717</v>
       </c>
     </row>
     <row r="44">
@@ -1613,7 +1841,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="n">
-        <v>38.0</v>
+        <v>1142.0</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
@@ -1622,10 +1850,10 @@
         <v>91</v>
       </c>
       <c r="E44" t="n">
-        <v>154300.0</v>
+        <v>715800.0</v>
       </c>
       <c r="F44" t="n">
-        <v>0.0017979966216097188</v>
+        <v>0.001954351448858275</v>
       </c>
     </row>
     <row r="45">
@@ -1633,7 +1861,7 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="n">
-        <v>197.0</v>
+        <v>1224.0</v>
       </c>
       <c r="C45" t="s">
         <v>92</v>
@@ -1642,10 +1870,10 @@
         <v>93</v>
       </c>
       <c r="E45" t="n">
-        <v>128300.0</v>
+        <v>3500000.0</v>
       </c>
       <c r="F45" t="n">
-        <v>0.001760910790208705</v>
+        <v>0.0018721873529803064</v>
       </c>
     </row>
     <row r="46">
@@ -1653,7 +1881,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="n">
-        <v>1214.0</v>
+        <v>1091.0</v>
       </c>
       <c r="C46" t="s">
         <v>94</v>
@@ -1662,10 +1890,10 @@
         <v>95</v>
       </c>
       <c r="E46" t="n">
-        <v>882500.0</v>
+        <v>1600000.0</v>
       </c>
       <c r="F46" t="n">
-        <v>0.001736943627979991</v>
+        <v>0.001872054558664358</v>
       </c>
     </row>
     <row r="47">
@@ -1673,7 +1901,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="n">
-        <v>13.0</v>
+        <v>1704.0</v>
       </c>
       <c r="C47" t="s">
         <v>96</v>
@@ -1682,10 +1910,10 @@
         <v>97</v>
       </c>
       <c r="E47" t="n">
-        <v>2800000.0</v>
+        <v>283300.0</v>
       </c>
       <c r="F47" t="n">
-        <v>0.0016889363937099989</v>
+        <v>0.0018589712746441517</v>
       </c>
     </row>
     <row r="48">
@@ -1693,7 +1921,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="n">
-        <v>1094.0</v>
+        <v>42.0</v>
       </c>
       <c r="C48" t="s">
         <v>98</v>
@@ -1702,10 +1930,10 @@
         <v>99</v>
       </c>
       <c r="E48" t="n">
-        <v>4300000.0</v>
+        <v>489700.0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0016662666325847858</v>
+        <v>0.001823477783290956</v>
       </c>
     </row>
     <row r="49">
@@ -1713,7 +1941,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="n">
-        <v>237.0</v>
+        <v>1250.0</v>
       </c>
       <c r="C49" t="s">
         <v>100</v>
@@ -1722,10 +1950,10 @@
         <v>101</v>
       </c>
       <c r="E49" t="n">
-        <v>373100.0</v>
+        <v>526600.0</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0016431924337497788</v>
+        <v>0.0017898805601969884</v>
       </c>
     </row>
     <row r="50">
@@ -1733,7 +1961,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="n">
-        <v>1200.0</v>
+        <v>1214.0</v>
       </c>
       <c r="C50" t="s">
         <v>102</v>
@@ -1742,10 +1970,10 @@
         <v>103</v>
       </c>
       <c r="E50" t="n">
-        <v>2000000.0</v>
+        <v>882500.0</v>
       </c>
       <c r="F50" t="n">
-        <v>0.0016175775338190144</v>
+        <v>0.0017730178899017573</v>
       </c>
     </row>
     <row r="51">
@@ -1753,7 +1981,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="n">
-        <v>1267.0</v>
+        <v>38.0</v>
       </c>
       <c r="C51" t="s">
         <v>104</v>
@@ -1762,10 +1990,10 @@
         <v>105</v>
       </c>
       <c r="E51" t="n">
-        <v>1100000.0</v>
+        <v>154300.0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0016041403653190072</v>
+        <v>0.0017531313561782477</v>
       </c>
     </row>
     <row r="52">
@@ -1773,7 +2001,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="n">
-        <v>243.0</v>
+        <v>47.0</v>
       </c>
       <c r="C52" t="s">
         <v>106</v>
@@ -1782,10 +2010,10 @@
         <v>107</v>
       </c>
       <c r="E52" t="n">
-        <v>250000.0</v>
+        <v>1300000.0</v>
       </c>
       <c r="F52" t="n">
-        <v>0.001603078805790848</v>
+        <v>0.001723732532964077</v>
       </c>
     </row>
     <row r="53">
@@ -1793,7 +2021,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="n">
-        <v>1151.0</v>
+        <v>1097.0</v>
       </c>
       <c r="C53" t="s">
         <v>108</v>
@@ -1802,10 +2030,10 @@
         <v>109</v>
       </c>
       <c r="E53" t="n">
-        <v>241400.0</v>
+        <v>1.04E7</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0015528722371484795</v>
+        <v>0.0017205734052560913</v>
       </c>
     </row>
     <row r="54">
@@ -1813,7 +2041,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="n">
-        <v>1373.0</v>
+        <v>1094.0</v>
       </c>
       <c r="C54" t="s">
         <v>110</v>
@@ -1822,10 +2050,10 @@
         <v>111</v>
       </c>
       <c r="E54" t="n">
-        <v>224500.0</v>
+        <v>4300000.0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0015297435081854484</v>
+        <v>0.00169847877624807</v>
       </c>
     </row>
     <row r="55">
@@ -1833,7 +2061,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="n">
-        <v>1103.0</v>
+        <v>1088.0</v>
       </c>
       <c r="C55" t="s">
         <v>112</v>
@@ -1842,10 +2070,10 @@
         <v>113</v>
       </c>
       <c r="E55" t="n">
-        <v>481900.0</v>
+        <v>404200.0</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0015197182853300512</v>
+        <v>0.001679291398945312</v>
       </c>
     </row>
     <row r="56">
@@ -1853,7 +2081,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="n">
-        <v>1131.0</v>
+        <v>1450.0</v>
       </c>
       <c r="C56" t="s">
         <v>114</v>
@@ -1862,10 +2090,10 @@
         <v>115</v>
       </c>
       <c r="E56" t="n">
-        <v>171000.0</v>
+        <v>1500000.0</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0014994390330214742</v>
+        <v>0.0016788737864152003</v>
       </c>
     </row>
     <row r="57">
@@ -1873,7 +2101,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="n">
-        <v>1118.0</v>
+        <v>43.0</v>
       </c>
       <c r="C57" t="s">
         <v>116</v>
@@ -1882,10 +2110,10 @@
         <v>117</v>
       </c>
       <c r="E57" t="n">
-        <v>157100.0</v>
+        <v>2900000.0</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0014487280912830044</v>
+        <v>0.0016524989444109133</v>
       </c>
     </row>
     <row r="58">
@@ -1893,7 +2121,7 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="n">
-        <v>1088.0</v>
+        <v>1146.0</v>
       </c>
       <c r="C58" t="s">
         <v>118</v>
@@ -1902,10 +2130,10 @@
         <v>119</v>
       </c>
       <c r="E58" t="n">
-        <v>404200.0</v>
+        <v>3700000.0</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0014303503662776705</v>
+        <v>0.0016484363559036421</v>
       </c>
     </row>
     <row r="59">
@@ -1913,7 +2141,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="n">
-        <v>1071.0</v>
+        <v>1820.0</v>
       </c>
       <c r="C59" t="s">
         <v>120</v>
@@ -1922,10 +2150,10 @@
         <v>121</v>
       </c>
       <c r="E59" t="n">
-        <v>6200000.0</v>
+        <v>473300.0</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0014122032438288342</v>
+        <v>0.001632981637670242</v>
       </c>
     </row>
     <row r="60">
@@ -1933,7 +2161,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="n">
-        <v>857.0</v>
+        <v>1211.0</v>
       </c>
       <c r="C60" t="s">
         <v>122</v>
@@ -1942,10 +2170,10 @@
         <v>123</v>
       </c>
       <c r="E60" t="n">
-        <v>3600000.0</v>
+        <v>100400.0</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0013882223858844144</v>
+        <v>0.0016267343654024352</v>
       </c>
     </row>
     <row r="61">
@@ -1953,7 +2181,7 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="n">
-        <v>47.0</v>
+        <v>1071.0</v>
       </c>
       <c r="C61" t="s">
         <v>124</v>
@@ -1962,10 +2190,10 @@
         <v>125</v>
       </c>
       <c r="E61" t="n">
-        <v>1300000.0</v>
+        <v>6200000.0</v>
       </c>
       <c r="F61" t="n">
-        <v>0.001385629149195842</v>
+        <v>0.001590163651984229</v>
       </c>
     </row>
     <row r="62">
@@ -1973,7 +2201,7 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="n">
-        <v>1287.0</v>
+        <v>857.0</v>
       </c>
       <c r="C62" t="s">
         <v>126</v>
@@ -1982,10 +2210,10 @@
         <v>127</v>
       </c>
       <c r="E62" t="n">
-        <v>163500.0</v>
+        <v>3600000.0</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0013476246982062816</v>
+        <v>0.0015888265288594864</v>
       </c>
     </row>
     <row r="63">
@@ -1993,7 +2221,7 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="n">
-        <v>337.0</v>
+        <v>1761.0</v>
       </c>
       <c r="C63" t="s">
         <v>128</v>
@@ -2002,10 +2230,10 @@
         <v>129</v>
       </c>
       <c r="E63" t="n">
-        <v>305300.0</v>
+        <v>921500.0</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0013415720456114435</v>
+        <v>0.0015840643703112908</v>
       </c>
     </row>
     <row r="64">
@@ -2013,7 +2241,7 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="n">
-        <v>104.0</v>
+        <v>1103.0</v>
       </c>
       <c r="C64" t="s">
         <v>130</v>
@@ -2022,10 +2250,10 @@
         <v>131</v>
       </c>
       <c r="E64" t="n">
-        <v>166400.0</v>
+        <v>481900.0</v>
       </c>
       <c r="F64" t="n">
-        <v>0.0013199299958167022</v>
+        <v>0.0015700537090585394</v>
       </c>
     </row>
     <row r="65">
@@ -2033,7 +2261,7 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="n">
-        <v>1222.0</v>
+        <v>1459.0</v>
       </c>
       <c r="C65" t="s">
         <v>132</v>
@@ -2042,10 +2270,10 @@
         <v>133</v>
       </c>
       <c r="E65" t="n">
-        <v>6700000.0</v>
+        <v>120300.0</v>
       </c>
       <c r="F65" t="n">
-        <v>0.001274501039360394</v>
+        <v>0.0015632565770225073</v>
       </c>
     </row>
     <row r="66">
@@ -2053,7 +2281,7 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="n">
-        <v>356.0</v>
+        <v>1616.0</v>
       </c>
       <c r="C66" t="s">
         <v>134</v>
@@ -2062,10 +2290,10 @@
         <v>135</v>
       </c>
       <c r="E66" t="n">
-        <v>245300.0</v>
+        <v>623000.0</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0012737059392460026</v>
+        <v>0.001514134481109672</v>
       </c>
     </row>
     <row r="67">
@@ -2073,7 +2301,7 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="n">
-        <v>158.0</v>
+        <v>1131.0</v>
       </c>
       <c r="C67" t="s">
         <v>136</v>
@@ -2082,10 +2310,10 @@
         <v>137</v>
       </c>
       <c r="E67" t="n">
-        <v>203900.0</v>
+        <v>171000.0</v>
       </c>
       <c r="F67" t="n">
-        <v>0.001265875038826276</v>
+        <v>0.001451077353538133</v>
       </c>
     </row>
     <row r="68">
@@ -2093,7 +2321,7 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="n">
-        <v>1207.0</v>
+        <v>337.0</v>
       </c>
       <c r="C68" t="s">
         <v>138</v>
@@ -2102,10 +2330,10 @@
         <v>139</v>
       </c>
       <c r="E68" t="n">
-        <v>787700.0</v>
+        <v>305300.0</v>
       </c>
       <c r="F68" t="n">
-        <v>0.0012595676793449525</v>
+        <v>0.00141766867577197</v>
       </c>
     </row>
     <row r="69">
@@ -2113,7 +2341,7 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="n">
-        <v>831.0</v>
+        <v>1695.0</v>
       </c>
       <c r="C69" t="s">
         <v>140</v>
@@ -2122,10 +2350,10 @@
         <v>141</v>
       </c>
       <c r="E69" t="n">
-        <v>4600000.0</v>
+        <v>206300.0</v>
       </c>
       <c r="F69" t="n">
-        <v>0.0012107825538423414</v>
+        <v>0.0013835259091622828</v>
       </c>
     </row>
     <row r="70">
@@ -2133,7 +2361,7 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="n">
-        <v>43.0</v>
+        <v>158.0</v>
       </c>
       <c r="C70" t="s">
         <v>142</v>
@@ -2142,10 +2370,10 @@
         <v>143</v>
       </c>
       <c r="E70" t="n">
-        <v>2900000.0</v>
+        <v>203900.0</v>
       </c>
       <c r="F70" t="n">
-        <v>0.001196127906606207</v>
+        <v>0.0013627286276510506</v>
       </c>
     </row>
     <row r="71">
@@ -2153,7 +2381,7 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="n">
-        <v>1127.0</v>
+        <v>1521.0</v>
       </c>
       <c r="C71" t="s">
         <v>144</v>
@@ -2162,10 +2390,10 @@
         <v>145</v>
       </c>
       <c r="E71" t="n">
-        <v>126300.0</v>
+        <v>774700.0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.0011562474271392669</v>
+        <v>0.0013614925636286552</v>
       </c>
     </row>
     <row r="72">
@@ -2173,7 +2401,7 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="n">
-        <v>1143.0</v>
+        <v>197.0</v>
       </c>
       <c r="C72" t="s">
         <v>146</v>
@@ -2182,10 +2410,10 @@
         <v>147</v>
       </c>
       <c r="E72" t="n">
-        <v>292300.0</v>
+        <v>128300.0</v>
       </c>
       <c r="F72" t="n">
-        <v>0.001120912224036289</v>
+        <v>0.0013155791241121636</v>
       </c>
     </row>
     <row r="73">
@@ -2193,7 +2421,7 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="n">
-        <v>1215.0</v>
+        <v>1118.0</v>
       </c>
       <c r="C73" t="s">
         <v>148</v>
@@ -2202,10 +2430,10 @@
         <v>149</v>
       </c>
       <c r="E73" t="n">
-        <v>1000000.0</v>
+        <v>157100.0</v>
       </c>
       <c r="F73" t="n">
-        <v>0.0011174144280672973</v>
+        <v>0.0012736516795337168</v>
       </c>
     </row>
     <row r="74">
@@ -2213,7 +2441,7 @@
         <v>73.0</v>
       </c>
       <c r="B74" t="n">
-        <v>1345.0</v>
+        <v>831.0</v>
       </c>
       <c r="C74" t="s">
         <v>150</v>
@@ -2222,10 +2450,10 @@
         <v>151</v>
       </c>
       <c r="E74" t="n">
-        <v>339700.0</v>
+        <v>4600000.0</v>
       </c>
       <c r="F74" t="n">
-        <v>0.0011081377768839824</v>
+        <v>0.001253258044898925</v>
       </c>
     </row>
     <row r="75">
@@ -2233,7 +2461,7 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="n">
-        <v>1170.0</v>
+        <v>20.0</v>
       </c>
       <c r="C75" t="s">
         <v>152</v>
@@ -2242,10 +2470,10 @@
         <v>153</v>
       </c>
       <c r="E75" t="n">
-        <v>184500.0</v>
+        <v>260500.0</v>
       </c>
       <c r="F75" t="n">
-        <v>0.0011061881768526353</v>
+        <v>0.001232554182008314</v>
       </c>
     </row>
     <row r="76">
@@ -2253,7 +2481,7 @@
         <v>75.0</v>
       </c>
       <c r="B76" t="n">
-        <v>835.0</v>
+        <v>1215.0</v>
       </c>
       <c r="C76" t="s">
         <v>154</v>
@@ -2262,10 +2490,10 @@
         <v>155</v>
       </c>
       <c r="E76" t="n">
-        <v>5400000.0</v>
+        <v>1000000.0</v>
       </c>
       <c r="F76" t="n">
-        <v>0.001103172323049124</v>
+        <v>0.0011953508402877673</v>
       </c>
     </row>
     <row r="77">
@@ -2273,7 +2501,7 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="n">
-        <v>257.0</v>
+        <v>1207.0</v>
       </c>
       <c r="C77" t="s">
         <v>156</v>
@@ -2282,10 +2510,10 @@
         <v>157</v>
       </c>
       <c r="E77" t="n">
-        <v>509800.0</v>
+        <v>787700.0</v>
       </c>
       <c r="F77" t="n">
-        <v>0.0010951128814964206</v>
+        <v>0.0011493503159746474</v>
       </c>
     </row>
     <row r="78">
@@ -2293,7 +2521,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" t="n">
-        <v>977.0</v>
+        <v>1127.0</v>
       </c>
       <c r="C78" t="s">
         <v>158</v>
@@ -2302,10 +2530,10 @@
         <v>159</v>
       </c>
       <c r="E78" t="n">
-        <v>146300.0</v>
+        <v>126300.0</v>
       </c>
       <c r="F78" t="n">
-        <v>0.0010659717538853211</v>
+        <v>0.0011347491789639721</v>
       </c>
     </row>
     <row r="79">
@@ -2313,7 +2541,7 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="n">
-        <v>1227.0</v>
+        <v>1418.0</v>
       </c>
       <c r="C79" t="s">
         <v>160</v>
@@ -2322,10 +2550,10 @@
         <v>161</v>
       </c>
       <c r="E79" t="n">
-        <v>2600000.0</v>
+        <v>799700.0</v>
       </c>
       <c r="F79" t="n">
-        <v>9.016087013055784E-4</v>
+        <v>0.0011223726098297652</v>
       </c>
     </row>
     <row r="80">
@@ -2333,7 +2561,7 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="n">
-        <v>1188.0</v>
+        <v>1408.0</v>
       </c>
       <c r="C80" t="s">
         <v>162</v>
@@ -2342,10 +2570,10 @@
         <v>163</v>
       </c>
       <c r="E80" t="n">
-        <v>167300.0</v>
+        <v>1300000.0</v>
       </c>
       <c r="F80" t="n">
-        <v>8.034813736907665E-4</v>
+        <v>0.0010688526361244048</v>
       </c>
     </row>
     <row r="81">
@@ -2353,7 +2581,7 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="n">
-        <v>1375.0</v>
+        <v>737.0</v>
       </c>
       <c r="C81" t="s">
         <v>164</v>
@@ -2362,10 +2590,10 @@
         <v>165</v>
       </c>
       <c r="E81" t="n">
-        <v>655400.0</v>
+        <v>231900.0</v>
       </c>
       <c r="F81" t="n">
-        <v>7.732668050072913E-4</v>
+        <v>0.0010620733622819455</v>
       </c>
     </row>
     <row r="82">
@@ -2373,7 +2601,7 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="n">
-        <v>1370.0</v>
+        <v>1720.0</v>
       </c>
       <c r="C82" t="s">
         <v>166</v>
@@ -2382,10 +2610,10 @@
         <v>167</v>
       </c>
       <c r="E82" t="n">
-        <v>879400.0</v>
+        <v>771800.0</v>
       </c>
       <c r="F82" t="n">
-        <v>7.109523900301872E-4</v>
+        <v>0.0010427164917134444</v>
       </c>
     </row>
     <row r="83">
@@ -2393,7 +2621,7 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="n">
-        <v>480.0</v>
+        <v>1733.0</v>
       </c>
       <c r="C83" t="s">
         <v>168</v>
@@ -2402,10 +2630,10 @@
         <v>169</v>
       </c>
       <c r="E83" t="n">
-        <v>417100.0</v>
+        <v>980900.0</v>
       </c>
       <c r="F83" t="n">
-        <v>6.978616099268195E-4</v>
+        <v>0.0010073471387427248</v>
       </c>
     </row>
     <row r="84">
@@ -2413,7 +2641,7 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="n">
-        <v>521.0</v>
+        <v>1287.0</v>
       </c>
       <c r="C84" t="s">
         <v>170</v>
@@ -2422,10 +2650,10 @@
         <v>171</v>
       </c>
       <c r="E84" t="n">
-        <v>113400.0</v>
+        <v>163500.0</v>
       </c>
       <c r="F84" t="n">
-        <v>6.866995290225996E-4</v>
+        <v>9.792374219651195E-4</v>
       </c>
     </row>
     <row r="85">
@@ -2433,7 +2661,7 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="n">
-        <v>983.0</v>
+        <v>835.0</v>
       </c>
       <c r="C85" t="s">
         <v>172</v>
@@ -2442,10 +2670,10 @@
         <v>173</v>
       </c>
       <c r="E85" t="n">
-        <v>3900000.0</v>
+        <v>5400000.0</v>
       </c>
       <c r="F85" t="n">
-        <v>6.814127128904875E-4</v>
+        <v>9.775431921414854E-4</v>
       </c>
     </row>
     <row r="86">
@@ -2453,7 +2681,7 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="n">
-        <v>495.0</v>
+        <v>1373.0</v>
       </c>
       <c r="C86" t="s">
         <v>174</v>
@@ -2462,10 +2690,10 @@
         <v>175</v>
       </c>
       <c r="E86" t="n">
-        <v>568300.0</v>
+        <v>224500.0</v>
       </c>
       <c r="F86" t="n">
-        <v>6.786566747672275E-4</v>
+        <v>9.714740326157219E-4</v>
       </c>
     </row>
     <row r="87">
@@ -2473,7 +2701,7 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="n">
-        <v>201.0</v>
+        <v>257.0</v>
       </c>
       <c r="C87" t="s">
         <v>176</v>
@@ -2482,10 +2710,10 @@
         <v>177</v>
       </c>
       <c r="E87" t="n">
-        <v>953900.0</v>
+        <v>509800.0</v>
       </c>
       <c r="F87" t="n">
-        <v>6.750808181028925E-4</v>
+        <v>9.659764951305276E-4</v>
       </c>
     </row>
     <row r="88">
@@ -2493,7 +2721,7 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="n">
-        <v>694.0</v>
+        <v>1484.0</v>
       </c>
       <c r="C88" t="s">
         <v>178</v>
@@ -2502,10 +2730,10 @@
         <v>179</v>
       </c>
       <c r="E88" t="n">
-        <v>641600.0</v>
+        <v>708600.0</v>
       </c>
       <c r="F88" t="n">
-        <v>6.725150160762309E-4</v>
+        <v>8.703558647705989E-4</v>
       </c>
     </row>
     <row r="89">
@@ -2513,7 +2741,7 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="n">
-        <v>188.0</v>
+        <v>356.0</v>
       </c>
       <c r="C89" t="s">
         <v>180</v>
@@ -2522,10 +2750,10 @@
         <v>181</v>
       </c>
       <c r="E89" t="n">
-        <v>178400.0</v>
+        <v>245300.0</v>
       </c>
       <c r="F89" t="n">
-        <v>6.459184495188411E-4</v>
+        <v>8.688722922538902E-4</v>
       </c>
     </row>
     <row r="90">
@@ -2533,7 +2761,7 @@
         <v>89.0</v>
       </c>
       <c r="B90" t="n">
-        <v>1265.0</v>
+        <v>1170.0</v>
       </c>
       <c r="C90" t="s">
         <v>182</v>
@@ -2542,10 +2770,10 @@
         <v>183</v>
       </c>
       <c r="E90" t="n">
-        <v>344700.0</v>
+        <v>184500.0</v>
       </c>
       <c r="F90" t="n">
-        <v>6.408919073195981E-4</v>
+        <v>8.523993362856956E-4</v>
       </c>
     </row>
     <row r="91">
@@ -2553,7 +2781,7 @@
         <v>90.0</v>
       </c>
       <c r="B91" t="n">
-        <v>767.0</v>
+        <v>983.0</v>
       </c>
       <c r="C91" t="s">
         <v>184</v>
@@ -2562,10 +2790,10 @@
         <v>185</v>
       </c>
       <c r="E91" t="n">
-        <v>190200.0</v>
+        <v>3900000.0</v>
       </c>
       <c r="F91" t="n">
-        <v>6.119973208890089E-4</v>
+        <v>8.495451233996868E-4</v>
       </c>
     </row>
     <row r="92">
@@ -2573,7 +2801,7 @@
         <v>91.0</v>
       </c>
       <c r="B92" t="n">
-        <v>1329.0</v>
+        <v>1375.0</v>
       </c>
       <c r="C92" t="s">
         <v>186</v>
@@ -2582,10 +2810,10 @@
         <v>187</v>
       </c>
       <c r="E92" t="n">
-        <v>345400.0</v>
+        <v>655400.0</v>
       </c>
       <c r="F92" t="n">
-        <v>5.866296680741851E-4</v>
+        <v>8.381584070491446E-4</v>
       </c>
     </row>
     <row r="93">
@@ -2593,7 +2821,7 @@
         <v>92.0</v>
       </c>
       <c r="B93" t="n">
-        <v>1369.0</v>
+        <v>188.0</v>
       </c>
       <c r="C93" t="s">
         <v>188</v>
@@ -2602,10 +2830,10 @@
         <v>189</v>
       </c>
       <c r="E93" t="n">
-        <v>3200000.0</v>
+        <v>178400.0</v>
       </c>
       <c r="F93" t="n">
-        <v>5.833192159847249E-4</v>
+        <v>8.212609628278664E-4</v>
       </c>
     </row>
     <row r="94">
@@ -2613,7 +2841,7 @@
         <v>93.0</v>
       </c>
       <c r="B94" t="n">
-        <v>241.0</v>
+        <v>1151.0</v>
       </c>
       <c r="C94" t="s">
         <v>190</v>
@@ -2622,10 +2850,10 @@
         <v>191</v>
       </c>
       <c r="E94" t="n">
-        <v>397600.0</v>
+        <v>241400.0</v>
       </c>
       <c r="F94" t="n">
-        <v>4.78525874593696E-4</v>
+        <v>8.157883707004251E-4</v>
       </c>
     </row>
     <row r="95">
@@ -2633,7 +2861,7 @@
         <v>94.0</v>
       </c>
       <c r="B95" t="n">
-        <v>91.0</v>
+        <v>1705.0</v>
       </c>
       <c r="C95" t="s">
         <v>192</v>
@@ -2642,10 +2870,10 @@
         <v>193</v>
       </c>
       <c r="E95" t="n">
-        <v>104400.0</v>
+        <v>1700000.0</v>
       </c>
       <c r="F95" t="n">
-        <v>4.3525069122627694E-4</v>
+        <v>8.119379022352219E-4</v>
       </c>
     </row>
     <row r="96">
@@ -2653,7 +2881,7 @@
         <v>95.0</v>
       </c>
       <c r="B96" t="n">
-        <v>268.0</v>
+        <v>694.0</v>
       </c>
       <c r="C96" t="s">
         <v>194</v>
@@ -2662,10 +2890,10 @@
         <v>195</v>
       </c>
       <c r="E96" t="n">
-        <v>592100.0</v>
+        <v>641600.0</v>
       </c>
       <c r="F96" t="n">
-        <v>4.18651607871494E-4</v>
+        <v>7.959117805538399E-4</v>
       </c>
     </row>
     <row r="97">
@@ -2673,7 +2901,7 @@
         <v>96.0</v>
       </c>
       <c r="B97" t="n">
-        <v>804.0</v>
+        <v>1329.0</v>
       </c>
       <c r="C97" t="s">
         <v>196</v>
@@ -2682,10 +2910,10 @@
         <v>197</v>
       </c>
       <c r="E97" t="n">
-        <v>298000.0</v>
+        <v>345400.0</v>
       </c>
       <c r="F97" t="n">
-        <v>4.009416310580277E-4</v>
+        <v>7.917452928736692E-4</v>
       </c>
     </row>
     <row r="98">
@@ -2693,7 +2921,7 @@
         <v>97.0</v>
       </c>
       <c r="B98" t="n">
-        <v>806.0</v>
+        <v>1188.0</v>
       </c>
       <c r="C98" t="s">
         <v>198</v>
@@ -2702,10 +2930,10 @@
         <v>199</v>
       </c>
       <c r="E98" t="n">
-        <v>140900.0</v>
+        <v>167300.0</v>
       </c>
       <c r="F98" t="n">
-        <v>3.819691626287385E-4</v>
+        <v>7.884939524311753E-4</v>
       </c>
     </row>
     <row r="99">
@@ -2713,7 +2941,7 @@
         <v>98.0</v>
       </c>
       <c r="B99" t="n">
-        <v>30.0</v>
+        <v>1572.0</v>
       </c>
       <c r="C99" t="s">
         <v>200</v>
@@ -2722,10 +2950,10 @@
         <v>201</v>
       </c>
       <c r="E99" t="n">
-        <v>241400.0</v>
+        <v>739000.0</v>
       </c>
       <c r="F99" t="n">
-        <v>3.7177144787178655E-4</v>
+        <v>7.612796294803964E-4</v>
       </c>
     </row>
     <row r="100">
@@ -2733,7 +2961,7 @@
         <v>99.0</v>
       </c>
       <c r="B100" t="n">
-        <v>361.0</v>
+        <v>1143.0</v>
       </c>
       <c r="C100" t="s">
         <v>202</v>
@@ -2742,10 +2970,10 @@
         <v>203</v>
       </c>
       <c r="E100" t="n">
-        <v>148300.0</v>
+        <v>292300.0</v>
       </c>
       <c r="F100" t="n">
-        <v>3.71685687634294E-4</v>
+        <v>7.488143004541795E-4</v>
       </c>
     </row>
     <row r="101">
@@ -2753,7 +2981,7 @@
         <v>100.0</v>
       </c>
       <c r="B101" t="n">
-        <v>302.0</v>
+        <v>243.0</v>
       </c>
       <c r="C101" t="s">
         <v>204</v>
@@ -2762,10 +2990,10 @@
         <v>205</v>
       </c>
       <c r="E101" t="n">
-        <v>198000.0</v>
+        <v>250000.0</v>
       </c>
       <c r="F101" t="n">
-        <v>3.580434759128908E-4</v>
+        <v>7.335476293186275E-4</v>
       </c>
     </row>
     <row r="102">
@@ -2773,7 +3001,7 @@
         <v>101.0</v>
       </c>
       <c r="B102" t="n">
-        <v>45.0</v>
+        <v>201.0</v>
       </c>
       <c r="C102" t="s">
         <v>206</v>
@@ -2782,10 +3010,10 @@
         <v>207</v>
       </c>
       <c r="E102" t="n">
-        <v>543000.0</v>
+        <v>953900.0</v>
       </c>
       <c r="F102" t="n">
-        <v>3.5768326879069795E-4</v>
+        <v>6.994758010624902E-4</v>
       </c>
     </row>
     <row r="103">
@@ -2793,7 +3021,7 @@
         <v>102.0</v>
       </c>
       <c r="B103" t="n">
-        <v>1332.0</v>
+        <v>1227.0</v>
       </c>
       <c r="C103" t="s">
         <v>208</v>
@@ -2802,10 +3030,10 @@
         <v>209</v>
       </c>
       <c r="E103" t="n">
-        <v>2900000.0</v>
+        <v>2600000.0</v>
       </c>
       <c r="F103" t="n">
-        <v>3.5578589650038506E-4</v>
+        <v>6.965170714553353E-4</v>
       </c>
     </row>
     <row r="104">
@@ -2813,7 +3041,7 @@
         <v>103.0</v>
       </c>
       <c r="B104" t="n">
-        <v>1317.0</v>
+        <v>521.0</v>
       </c>
       <c r="C104" t="s">
         <v>210</v>
@@ -2822,10 +3050,10 @@
         <v>211</v>
       </c>
       <c r="E104" t="n">
-        <v>818600.0</v>
+        <v>113400.0</v>
       </c>
       <c r="F104" t="n">
-        <v>3.457068547214898E-4</v>
+        <v>6.914712887067364E-4</v>
       </c>
     </row>
     <row r="105">
@@ -2833,7 +3061,7 @@
         <v>104.0</v>
       </c>
       <c r="B105" t="n">
-        <v>737.0</v>
+        <v>1474.0</v>
       </c>
       <c r="C105" t="s">
         <v>212</v>
@@ -2842,10 +3070,10 @@
         <v>213</v>
       </c>
       <c r="E105" t="n">
-        <v>231900.0</v>
+        <v>718000.0</v>
       </c>
       <c r="F105" t="n">
-        <v>3.189835653678551E-4</v>
+        <v>6.760390182378994E-4</v>
       </c>
     </row>
     <row r="106">
@@ -2853,7 +3081,7 @@
         <v>105.0</v>
       </c>
       <c r="B106" t="n">
-        <v>428.0</v>
+        <v>1345.0</v>
       </c>
       <c r="C106" t="s">
         <v>214</v>
@@ -2862,10 +3090,10 @@
         <v>215</v>
       </c>
       <c r="E106" t="n">
-        <v>310700.0</v>
+        <v>339700.0</v>
       </c>
       <c r="F106" t="n">
-        <v>2.8477497509138904E-4</v>
+        <v>6.699568571121922E-4</v>
       </c>
     </row>
     <row r="107">
@@ -2873,7 +3101,7 @@
         <v>106.0</v>
       </c>
       <c r="B107" t="n">
-        <v>440.0</v>
+        <v>1369.0</v>
       </c>
       <c r="C107" t="s">
         <v>216</v>
@@ -2882,10 +3110,10 @@
         <v>217</v>
       </c>
       <c r="E107" t="n">
-        <v>702500.0</v>
+        <v>3200000.0</v>
       </c>
       <c r="F107" t="n">
-        <v>2.530105424830382E-4</v>
+        <v>6.64150999277202E-4</v>
       </c>
     </row>
     <row r="108">
@@ -2893,7 +3121,7 @@
         <v>107.0</v>
       </c>
       <c r="B108" t="n">
-        <v>103.0</v>
+        <v>1817.0</v>
       </c>
       <c r="C108" t="s">
         <v>218</v>
@@ -2902,10 +3130,10 @@
         <v>219</v>
       </c>
       <c r="E108" t="n">
-        <v>1000000.0</v>
+        <v>106700.0</v>
       </c>
       <c r="F108" t="n">
-        <v>2.479349073592222E-4</v>
+        <v>6.112910218844614E-4</v>
       </c>
     </row>
     <row r="109">
@@ -2913,7 +3141,7 @@
         <v>108.0</v>
       </c>
       <c r="B109" t="n">
-        <v>978.0</v>
+        <v>1721.0</v>
       </c>
       <c r="C109" t="s">
         <v>220</v>
@@ -2922,10 +3150,10 @@
         <v>221</v>
       </c>
       <c r="E109" t="n">
-        <v>1700000.0</v>
+        <v>217200.0</v>
       </c>
       <c r="F109" t="n">
-        <v>2.4326588710414732E-4</v>
+        <v>6.044175350063325E-4</v>
       </c>
     </row>
     <row r="110">
@@ -2933,7 +3161,7 @@
         <v>109.0</v>
       </c>
       <c r="B110" t="n">
-        <v>151.0</v>
+        <v>1265.0</v>
       </c>
       <c r="C110" t="s">
         <v>222</v>
@@ -2942,10 +3170,10 @@
         <v>223</v>
       </c>
       <c r="E110" t="n">
-        <v>200300.0</v>
+        <v>344700.0</v>
       </c>
       <c r="F110" t="n">
-        <v>2.3341888307889212E-4</v>
+        <v>5.928019609771056E-4</v>
       </c>
     </row>
     <row r="111">
@@ -2953,7 +3181,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" t="n">
-        <v>72.0</v>
+        <v>1799.0</v>
       </c>
       <c r="C111" t="s">
         <v>224</v>
@@ -2962,10 +3190,770 @@
         <v>225</v>
       </c>
       <c r="E111" t="n">
+        <v>4099999.0</v>
+      </c>
+      <c r="F111" t="n">
+        <v>5.882728026775615E-4</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="B112" t="n">
+        <v>978.0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>226</v>
+      </c>
+      <c r="D112" t="s">
+        <v>227</v>
+      </c>
+      <c r="E112" t="n">
+        <v>1700000.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>5.825907720455717E-4</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="B113" t="n">
+        <v>495.0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>228</v>
+      </c>
+      <c r="D113" t="s">
+        <v>229</v>
+      </c>
+      <c r="E113" t="n">
+        <v>568300.0</v>
+      </c>
+      <c r="F113" t="n">
+        <v>5.519609269422852E-4</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="B114" t="n">
+        <v>1562.0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>230</v>
+      </c>
+      <c r="D114" t="s">
+        <v>231</v>
+      </c>
+      <c r="E114" t="n">
+        <v>421100.0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>5.473147051879729E-4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="B115" t="n">
+        <v>1414.0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>232</v>
+      </c>
+      <c r="D115" t="s">
+        <v>233</v>
+      </c>
+      <c r="E115" t="n">
+        <v>200900.0</v>
+      </c>
+      <c r="F115" t="n">
+        <v>4.6813514756974104E-4</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="B116" t="n">
+        <v>1736.0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>234</v>
+      </c>
+      <c r="D116" t="s">
+        <v>235</v>
+      </c>
+      <c r="E116" t="n">
+        <v>297400.0</v>
+      </c>
+      <c r="F116" t="n">
+        <v>4.678172231155743E-4</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="B117" t="n">
+        <v>767.0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>236</v>
+      </c>
+      <c r="D117" t="s">
+        <v>237</v>
+      </c>
+      <c r="E117" t="n">
+        <v>190200.0</v>
+      </c>
+      <c r="F117" t="n">
+        <v>4.6636440663613496E-4</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="B118" t="n">
+        <v>1370.0</v>
+      </c>
+      <c r="C118" t="s">
+        <v>238</v>
+      </c>
+      <c r="D118" t="s">
+        <v>239</v>
+      </c>
+      <c r="E118" t="n">
+        <v>879400.0</v>
+      </c>
+      <c r="F118" t="n">
+        <v>4.5877666120444443E-4</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="B119" t="n">
+        <v>1332.0</v>
+      </c>
+      <c r="C119" t="s">
+        <v>240</v>
+      </c>
+      <c r="D119" t="s">
+        <v>241</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2900000.0</v>
+      </c>
+      <c r="F119" t="n">
+        <v>4.5850428815390366E-4</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119.0</v>
+      </c>
+      <c r="B120" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="C120" t="s">
+        <v>242</v>
+      </c>
+      <c r="D120" t="s">
+        <v>243</v>
+      </c>
+      <c r="E120" t="n">
+        <v>104400.0</v>
+      </c>
+      <c r="F120" t="n">
+        <v>4.579616545909109E-4</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="B121" t="n">
+        <v>1655.0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>244</v>
+      </c>
+      <c r="D121" t="s">
+        <v>245</v>
+      </c>
+      <c r="E121" t="n">
+        <v>616500.0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>4.397991803864941E-4</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="B122" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>246</v>
+      </c>
+      <c r="D122" t="s">
+        <v>247</v>
+      </c>
+      <c r="E122" t="n">
+        <v>1000000.0</v>
+      </c>
+      <c r="F122" t="n">
+        <v>4.329093386942924E-4</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="B123" t="n">
+        <v>977.0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>248</v>
+      </c>
+      <c r="D123" t="s">
+        <v>249</v>
+      </c>
+      <c r="E123" t="n">
+        <v>146300.0</v>
+      </c>
+      <c r="F123" t="n">
+        <v>3.71938363596416E-4</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="B124" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>250</v>
+      </c>
+      <c r="D124" t="s">
+        <v>251</v>
+      </c>
+      <c r="E124" t="n">
+        <v>543000.0</v>
+      </c>
+      <c r="F124" t="n">
+        <v>3.7117770446994645E-4</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="B125" t="n">
+        <v>806.0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>252</v>
+      </c>
+      <c r="D125" t="s">
+        <v>253</v>
+      </c>
+      <c r="E125" t="n">
+        <v>140900.0</v>
+      </c>
+      <c r="F125" t="n">
+        <v>3.6924687596684734E-4</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="B126" t="n">
+        <v>1523.0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>254</v>
+      </c>
+      <c r="D126" t="s">
+        <v>255</v>
+      </c>
+      <c r="E126" t="n">
+        <v>226500.0</v>
+      </c>
+      <c r="F126" t="n">
+        <v>3.6910613930589507E-4</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="B127" t="n">
+        <v>480.0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>256</v>
+      </c>
+      <c r="D127" t="s">
+        <v>257</v>
+      </c>
+      <c r="E127" t="n">
+        <v>417100.0</v>
+      </c>
+      <c r="F127" t="n">
+        <v>3.612972123499437E-4</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1567.0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>258</v>
+      </c>
+      <c r="D128" t="s">
+        <v>259</v>
+      </c>
+      <c r="E128" t="n">
+        <v>129199.0</v>
+      </c>
+      <c r="F128" t="n">
+        <v>3.3078517250830517E-4</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="B129" t="n">
+        <v>845.0</v>
+      </c>
+      <c r="C129" t="s">
+        <v>260</v>
+      </c>
+      <c r="D129" t="s">
+        <v>261</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1100000.0</v>
+      </c>
+      <c r="F129" t="n">
+        <v>3.259186644960659E-4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="B130" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="C130" t="s">
+        <v>262</v>
+      </c>
+      <c r="D130" t="s">
+        <v>263</v>
+      </c>
+      <c r="E130" t="n">
+        <v>241400.0</v>
+      </c>
+      <c r="F130" t="n">
+        <v>3.237930652699846E-4</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="B131" t="n">
+        <v>268.0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>264</v>
+      </c>
+      <c r="D131" t="s">
+        <v>265</v>
+      </c>
+      <c r="E131" t="n">
+        <v>592100.0</v>
+      </c>
+      <c r="F131" t="n">
+        <v>3.002867063196743E-4</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131.0</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1812.0</v>
+      </c>
+      <c r="C132" t="s">
+        <v>266</v>
+      </c>
+      <c r="D132" t="s">
+        <v>267</v>
+      </c>
+      <c r="E132" t="n">
+        <v>182500.0</v>
+      </c>
+      <c r="F132" t="n">
+        <v>2.689453938318088E-4</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="B133" t="n">
+        <v>804.0</v>
+      </c>
+      <c r="C133" t="s">
+        <v>268</v>
+      </c>
+      <c r="D133" t="s">
+        <v>269</v>
+      </c>
+      <c r="E133" t="n">
+        <v>298000.0</v>
+      </c>
+      <c r="F133" t="n">
+        <v>2.5675784806850624E-4</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>133.0</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1403.0</v>
+      </c>
+      <c r="C134" t="s">
+        <v>270</v>
+      </c>
+      <c r="D134" t="s">
+        <v>271</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1.14E8</v>
+      </c>
+      <c r="F134" t="n">
+        <v>2.3375602914346127E-4</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>134.0</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1678.0</v>
+      </c>
+      <c r="C135" t="s">
+        <v>272</v>
+      </c>
+      <c r="D135" t="s">
+        <v>273</v>
+      </c>
+      <c r="E135" t="n">
+        <v>212000.0</v>
+      </c>
+      <c r="F135" t="n">
+        <v>2.3067477293696424E-4</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>135.0</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1317.0</v>
+      </c>
+      <c r="C136" t="s">
+        <v>274</v>
+      </c>
+      <c r="D136" t="s">
+        <v>275</v>
+      </c>
+      <c r="E136" t="n">
+        <v>818600.0</v>
+      </c>
+      <c r="F136" t="n">
+        <v>2.2331413078220452E-4</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>136.0</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1700.0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>276</v>
+      </c>
+      <c r="D137" t="s">
+        <v>277</v>
+      </c>
+      <c r="E137" t="n">
+        <v>2200000.0</v>
+      </c>
+      <c r="F137" t="n">
+        <v>2.1600474815771016E-4</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>137.0</v>
+      </c>
+      <c r="B138" t="n">
+        <v>241.0</v>
+      </c>
+      <c r="C138" t="s">
+        <v>278</v>
+      </c>
+      <c r="D138" t="s">
+        <v>279</v>
+      </c>
+      <c r="E138" t="n">
+        <v>397600.0</v>
+      </c>
+      <c r="F138" t="n">
+        <v>2.09932177367979E-4</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="B139" t="n">
+        <v>361.0</v>
+      </c>
+      <c r="C139" t="s">
+        <v>280</v>
+      </c>
+      <c r="D139" t="s">
+        <v>281</v>
+      </c>
+      <c r="E139" t="n">
+        <v>148300.0</v>
+      </c>
+      <c r="F139" t="n">
+        <v>2.09932177367979E-4</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="B140" t="n">
+        <v>302.0</v>
+      </c>
+      <c r="C140" t="s">
+        <v>282</v>
+      </c>
+      <c r="D140" t="s">
+        <v>283</v>
+      </c>
+      <c r="E140" t="n">
+        <v>198000.0</v>
+      </c>
+      <c r="F140" t="n">
+        <v>2.0863773391134068E-4</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="B141" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="C141" t="s">
+        <v>284</v>
+      </c>
+      <c r="D141" t="s">
+        <v>285</v>
+      </c>
+      <c r="E141" t="n">
         <v>186300.0</v>
       </c>
-      <c r="F111" t="n">
-        <v>1.947755786594391E-4</v>
+      <c r="F141" t="n">
+        <v>2.0270678946056043E-4</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>141.0</v>
+      </c>
+      <c r="B142" t="n">
+        <v>1781.0</v>
+      </c>
+      <c r="C142" t="s">
+        <v>286</v>
+      </c>
+      <c r="D142" t="s">
+        <v>287</v>
+      </c>
+      <c r="E142" t="n">
+        <v>240600.0</v>
+      </c>
+      <c r="F142" t="n">
+        <v>1.7203556546127168E-4</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>142.0</v>
+      </c>
+      <c r="B143" t="n">
+        <v>428.0</v>
+      </c>
+      <c r="C143" t="s">
+        <v>288</v>
+      </c>
+      <c r="D143" t="s">
+        <v>289</v>
+      </c>
+      <c r="E143" t="n">
+        <v>310700.0</v>
+      </c>
+      <c r="F143" t="n">
+        <v>1.5288645500859257E-4</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>143.0</v>
+      </c>
+      <c r="B144" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="C144" t="s">
+        <v>290</v>
+      </c>
+      <c r="D144" t="s">
+        <v>291</v>
+      </c>
+      <c r="E144" t="n">
+        <v>200300.0</v>
+      </c>
+      <c r="F144" t="n">
+        <v>1.518116840856357E-4</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1536.0</v>
+      </c>
+      <c r="C145" t="s">
+        <v>292</v>
+      </c>
+      <c r="D145" t="s">
+        <v>293</v>
+      </c>
+      <c r="E145" t="n">
+        <v>708500.0</v>
+      </c>
+      <c r="F145" t="n">
+        <v>1.4399025920575732E-4</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>145.0</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1531.0</v>
+      </c>
+      <c r="C146" t="s">
+        <v>294</v>
+      </c>
+      <c r="D146" t="s">
+        <v>295</v>
+      </c>
+      <c r="E146" t="n">
+        <v>189900.0</v>
+      </c>
+      <c r="F146" t="n">
+        <v>1.2070959706834313E-4</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="B147" t="n">
+        <v>440.0</v>
+      </c>
+      <c r="C147" t="s">
+        <v>296</v>
+      </c>
+      <c r="D147" t="s">
+        <v>297</v>
+      </c>
+      <c r="E147" t="n">
+        <v>702500.0</v>
+      </c>
+      <c r="F147" t="n">
+        <v>1.2070959706834313E-4</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>147.0</v>
+      </c>
+      <c r="B148" t="n">
+        <v>1564.0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>298</v>
+      </c>
+      <c r="D148" t="s">
+        <v>299</v>
+      </c>
+      <c r="E148" t="n">
+        <v>931200.0</v>
+      </c>
+      <c r="F148" t="n">
+        <v>1.2070959706834313E-4</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>148.0</v>
+      </c>
+      <c r="B149" t="n">
+        <v>1550.0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>300</v>
+      </c>
+      <c r="D149" t="s">
+        <v>301</v>
+      </c>
+      <c r="E149" t="n">
+        <v>159900.0</v>
+      </c>
+      <c r="F149" t="n">
+        <v>1.2070959706834313E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>